<commit_message>
Bug-fix. Revision of the entire documents.
</commit_message>
<xml_diff>
--- a/Analysis/centroids_allquestions.xlsx
+++ b/Analysis/centroids_allquestions.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-8140" yWindow="-28340" windowWidth="24060" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24060" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Distances" sheetId="1" r:id="rId1"/>
     <sheet name="Distances_Testes Estatisticos" sheetId="13" r:id="rId2"/>
-    <sheet name="Difficulty" sheetId="14" r:id="rId3"/>
-    <sheet name="Demo - Genders" sheetId="16" r:id="rId4"/>
+    <sheet name="Plan1" sheetId="17" r:id="rId3"/>
+    <sheet name="Difficulty" sheetId="14" r:id="rId4"/>
+    <sheet name="Demo - Genders" sheetId="16" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="203">
   <si>
     <t>Question 1</t>
   </si>
@@ -573,6 +574,69 @@
   </si>
   <si>
     <t>FRIEDMAN LAB - UNCAL</t>
+  </si>
+  <si>
+    <t>Count Pairs</t>
+  </si>
+  <si>
+    <t>Count Individual</t>
+  </si>
+  <si>
+    <t>Reference Pair</t>
+  </si>
+  <si>
+    <t>Most Given Values</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>G (141)</t>
+  </si>
+  <si>
+    <t>R (93)</t>
+  </si>
+  <si>
+    <t>B (13)</t>
+  </si>
+  <si>
+    <t>R-G (56)</t>
+  </si>
+  <si>
+    <t>G-G (31)</t>
+  </si>
+  <si>
+    <t>G-B (11)</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Cyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red </t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>R (117)</t>
+  </si>
+  <si>
+    <t>B (52)</t>
+  </si>
+  <si>
+    <t>Pink (52)</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1192,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1302,8 +1366,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="399">
+  <cellXfs count="402">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1984,74 +2052,206 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2059,158 +2259,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="177">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2297,6 +2374,8 @@
     <cellStyle name="Hiperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -2383,6 +2462,8 @@
     <cellStyle name="Hiperlink Visitado" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2674,36 +2755,36 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="334" t="s">
+      <c r="B1" s="328" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="334"/>
-      <c r="D1" s="334"/>
-      <c r="E1" s="334"/>
-      <c r="F1" s="334"/>
-      <c r="G1" s="334"/>
-      <c r="H1" s="334"/>
-      <c r="I1" s="334"/>
-      <c r="J1" s="334"/>
-      <c r="K1" s="334"/>
-      <c r="L1" s="334"/>
-      <c r="M1" s="334"/>
-      <c r="N1" s="334"/>
-      <c r="O1" s="334"/>
+      <c r="C1" s="328"/>
+      <c r="D1" s="328"/>
+      <c r="E1" s="328"/>
+      <c r="F1" s="328"/>
+      <c r="G1" s="328"/>
+      <c r="H1" s="328"/>
+      <c r="I1" s="328"/>
+      <c r="J1" s="328"/>
+      <c r="K1" s="328"/>
+      <c r="L1" s="328"/>
+      <c r="M1" s="328"/>
+      <c r="N1" s="328"/>
+      <c r="O1" s="328"/>
       <c r="P1" s="2"/>
-      <c r="S1" s="326" t="s">
+      <c r="S1" s="330" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="326"/>
-      <c r="U1" s="326"/>
-      <c r="V1" s="326"/>
-      <c r="W1" s="326"/>
-      <c r="X1" s="326"/>
-      <c r="Y1" s="326"/>
-      <c r="Z1" s="326"/>
-      <c r="AA1" s="326"/>
-      <c r="AB1" s="326"/>
-      <c r="AC1" s="326"/>
+      <c r="T1" s="330"/>
+      <c r="U1" s="330"/>
+      <c r="V1" s="330"/>
+      <c r="W1" s="330"/>
+      <c r="X1" s="330"/>
+      <c r="Y1" s="330"/>
+      <c r="Z1" s="330"/>
+      <c r="AA1" s="330"/>
+      <c r="AB1" s="330"/>
+      <c r="AC1" s="330"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -2731,21 +2812,21 @@
         <v>21</v>
       </c>
       <c r="O2" s="337"/>
-      <c r="P2" s="325"/>
-      <c r="T2" s="326" t="s">
+      <c r="P2" s="338"/>
+      <c r="T2" s="330" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="326"/>
-      <c r="V2" s="326"/>
-      <c r="W2" s="326"/>
-      <c r="X2" s="326"/>
-      <c r="Y2" s="326" t="s">
+      <c r="U2" s="330"/>
+      <c r="V2" s="330"/>
+      <c r="W2" s="330"/>
+      <c r="X2" s="330"/>
+      <c r="Y2" s="330" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="326"/>
-      <c r="AA2" s="326"/>
-      <c r="AB2" s="326"/>
-      <c r="AC2" s="326"/>
+      <c r="Z2" s="330"/>
+      <c r="AA2" s="330"/>
+      <c r="AB2" s="330"/>
+      <c r="AC2" s="330"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -3491,95 +3572,95 @@
     <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="334" t="s">
+      <c r="B22" s="328" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="334"/>
-      <c r="D22" s="334"/>
-      <c r="E22" s="334"/>
-      <c r="F22" s="334"/>
-      <c r="G22" s="334"/>
-      <c r="H22" s="334"/>
-      <c r="I22" s="334"/>
-      <c r="J22" s="334"/>
-      <c r="K22" s="334"/>
-      <c r="L22" s="334"/>
-      <c r="M22" s="334"/>
-      <c r="N22" s="334"/>
-      <c r="O22" s="334"/>
+      <c r="C22" s="328"/>
+      <c r="D22" s="328"/>
+      <c r="E22" s="328"/>
+      <c r="F22" s="328"/>
+      <c r="G22" s="328"/>
+      <c r="H22" s="328"/>
+      <c r="I22" s="328"/>
+      <c r="J22" s="328"/>
+      <c r="K22" s="328"/>
+      <c r="L22" s="328"/>
+      <c r="M22" s="328"/>
+      <c r="N22" s="328"/>
+      <c r="O22" s="328"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="331" t="s">
+      <c r="S22" s="336" t="s">
         <v>51</v>
       </c>
-      <c r="T22" s="331"/>
-      <c r="U22" s="331"/>
-      <c r="V22" s="331"/>
-      <c r="W22" s="331"/>
-      <c r="X22" s="331"/>
-      <c r="Y22" s="331"/>
-      <c r="Z22" s="331"/>
-      <c r="AA22" s="331"/>
-      <c r="AB22" s="331"/>
-      <c r="AC22" s="331"/>
-      <c r="AD22" s="331"/>
-      <c r="AE22" s="331"/>
-      <c r="AF22" s="331"/>
+      <c r="T22" s="336"/>
+      <c r="U22" s="336"/>
+      <c r="V22" s="336"/>
+      <c r="W22" s="336"/>
+      <c r="X22" s="336"/>
+      <c r="Y22" s="336"/>
+      <c r="Z22" s="336"/>
+      <c r="AA22" s="336"/>
+      <c r="AB22" s="336"/>
+      <c r="AC22" s="336"/>
+      <c r="AD22" s="336"/>
+      <c r="AE22" s="336"/>
+      <c r="AF22" s="336"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="332" t="s">
+      <c r="B23" s="339" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="332"/>
-      <c r="D23" s="332"/>
-      <c r="E23" s="332" t="s">
+      <c r="C23" s="339"/>
+      <c r="D23" s="339"/>
+      <c r="E23" s="339" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="332"/>
-      <c r="G23" s="332"/>
-      <c r="H23" s="332" t="s">
+      <c r="F23" s="339"/>
+      <c r="G23" s="339"/>
+      <c r="H23" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="332"/>
-      <c r="J23" s="332"/>
-      <c r="K23" s="332" t="s">
+      <c r="I23" s="339"/>
+      <c r="J23" s="339"/>
+      <c r="K23" s="339" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="332"/>
-      <c r="M23" s="332"/>
-      <c r="N23" s="332" t="s">
+      <c r="L23" s="339"/>
+      <c r="M23" s="339"/>
+      <c r="N23" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="332"/>
-      <c r="P23" s="333"/>
+      <c r="O23" s="339"/>
+      <c r="P23" s="340"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="332" t="s">
+      <c r="S23" s="339" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="332"/>
-      <c r="U23" s="332"/>
-      <c r="V23" s="332" t="s">
+      <c r="T23" s="339"/>
+      <c r="U23" s="339"/>
+      <c r="V23" s="339" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="332"/>
-      <c r="X23" s="332"/>
-      <c r="Y23" s="332" t="s">
+      <c r="W23" s="339"/>
+      <c r="X23" s="339"/>
+      <c r="Y23" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="332"/>
-      <c r="AA23" s="332"/>
-      <c r="AB23" s="332" t="s">
+      <c r="Z23" s="339"/>
+      <c r="AA23" s="339"/>
+      <c r="AB23" s="339" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="332"/>
-      <c r="AD23" s="332"/>
-      <c r="AE23" s="332" t="s">
+      <c r="AC23" s="339"/>
+      <c r="AD23" s="339"/>
+      <c r="AE23" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="332"/>
-      <c r="AG23" s="333"/>
+      <c r="AF23" s="339"/>
+      <c r="AG23" s="340"/>
     </row>
     <row r="24" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -4663,159 +4744,159 @@
     <row r="42" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="331" t="s">
+      <c r="B43" s="336" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="331"/>
-      <c r="D43" s="331"/>
-      <c r="E43" s="331"/>
-      <c r="F43" s="331"/>
-      <c r="G43" s="331"/>
-      <c r="H43" s="331"/>
-      <c r="I43" s="331"/>
-      <c r="J43" s="331"/>
-      <c r="K43" s="331"/>
-      <c r="L43" s="331"/>
-      <c r="M43" s="331"/>
-      <c r="N43" s="331"/>
-      <c r="O43" s="331"/>
-      <c r="P43" s="331"/>
+      <c r="C43" s="336"/>
+      <c r="D43" s="336"/>
+      <c r="E43" s="336"/>
+      <c r="F43" s="336"/>
+      <c r="G43" s="336"/>
+      <c r="H43" s="336"/>
+      <c r="I43" s="336"/>
+      <c r="J43" s="336"/>
+      <c r="K43" s="336"/>
+      <c r="L43" s="336"/>
+      <c r="M43" s="336"/>
+      <c r="N43" s="336"/>
+      <c r="O43" s="336"/>
+      <c r="P43" s="336"/>
       <c r="Q43" s="45"/>
       <c r="R43" s="45"/>
       <c r="S43" s="46"/>
       <c r="T43" s="335" t="s">
         <v>53</v>
       </c>
-      <c r="U43" s="331"/>
-      <c r="V43" s="331"/>
-      <c r="W43" s="331"/>
-      <c r="X43" s="331"/>
-      <c r="Y43" s="331"/>
-      <c r="Z43" s="331"/>
-      <c r="AA43" s="331"/>
-      <c r="AB43" s="331"/>
-      <c r="AC43" s="331"/>
-      <c r="AD43" s="331"/>
-      <c r="AE43" s="331"/>
-      <c r="AF43" s="331"/>
-      <c r="AG43" s="331"/>
-      <c r="AH43" s="331"/>
+      <c r="U43" s="336"/>
+      <c r="V43" s="336"/>
+      <c r="W43" s="336"/>
+      <c r="X43" s="336"/>
+      <c r="Y43" s="336"/>
+      <c r="Z43" s="336"/>
+      <c r="AA43" s="336"/>
+      <c r="AB43" s="336"/>
+      <c r="AC43" s="336"/>
+      <c r="AD43" s="336"/>
+      <c r="AE43" s="336"/>
+      <c r="AF43" s="336"/>
+      <c r="AG43" s="336"/>
+      <c r="AH43" s="336"/>
       <c r="AI43" s="45"/>
       <c r="AJ43" s="45"/>
       <c r="AK43" s="46"/>
       <c r="AL43" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="AM43" s="331"/>
-      <c r="AN43" s="331"/>
-      <c r="AO43" s="331"/>
-      <c r="AP43" s="331"/>
-      <c r="AQ43" s="331"/>
-      <c r="AR43" s="331"/>
-      <c r="AS43" s="331"/>
-      <c r="AT43" s="331"/>
-      <c r="AU43" s="331"/>
-      <c r="AV43" s="331"/>
-      <c r="AW43" s="331"/>
-      <c r="AX43" s="331"/>
-      <c r="AY43" s="331"/>
-      <c r="AZ43" s="331"/>
+      <c r="AM43" s="336"/>
+      <c r="AN43" s="336"/>
+      <c r="AO43" s="336"/>
+      <c r="AP43" s="336"/>
+      <c r="AQ43" s="336"/>
+      <c r="AR43" s="336"/>
+      <c r="AS43" s="336"/>
+      <c r="AT43" s="336"/>
+      <c r="AU43" s="336"/>
+      <c r="AV43" s="336"/>
+      <c r="AW43" s="336"/>
+      <c r="AX43" s="336"/>
+      <c r="AY43" s="336"/>
+      <c r="AZ43" s="336"/>
       <c r="BA43" s="47"/>
       <c r="BB43" s="47"/>
       <c r="BC43" s="48"/>
     </row>
     <row r="44" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-      <c r="B44" s="343" t="s">
+      <c r="B44" s="345" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="343"/>
-      <c r="D44" s="343"/>
-      <c r="E44" s="340" t="s">
+      <c r="C44" s="345"/>
+      <c r="D44" s="345"/>
+      <c r="E44" s="342" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="340"/>
-      <c r="G44" s="340"/>
-      <c r="H44" s="340" t="s">
+      <c r="F44" s="342"/>
+      <c r="G44" s="342"/>
+      <c r="H44" s="342" t="s">
         <v>18</v>
       </c>
-      <c r="I44" s="340"/>
-      <c r="J44" s="340"/>
-      <c r="K44" s="341" t="s">
+      <c r="I44" s="342"/>
+      <c r="J44" s="342"/>
+      <c r="K44" s="343" t="s">
         <v>19</v>
       </c>
-      <c r="L44" s="332"/>
-      <c r="M44" s="342"/>
-      <c r="N44" s="340" t="s">
+      <c r="L44" s="339"/>
+      <c r="M44" s="344"/>
+      <c r="N44" s="342" t="s">
         <v>20</v>
       </c>
-      <c r="O44" s="340"/>
-      <c r="P44" s="340"/>
-      <c r="Q44" s="332" t="s">
+      <c r="O44" s="342"/>
+      <c r="P44" s="342"/>
+      <c r="Q44" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="R44" s="332"/>
-      <c r="S44" s="333"/>
-      <c r="T44" s="336" t="s">
+      <c r="R44" s="339"/>
+      <c r="S44" s="340"/>
+      <c r="T44" s="346" t="s">
         <v>45</v>
       </c>
       <c r="U44" s="337"/>
       <c r="V44" s="337"/>
-      <c r="W44" s="332" t="s">
+      <c r="W44" s="339" t="s">
         <v>17</v>
       </c>
-      <c r="X44" s="332"/>
-      <c r="Y44" s="332"/>
-      <c r="Z44" s="332" t="s">
+      <c r="X44" s="339"/>
+      <c r="Y44" s="339"/>
+      <c r="Z44" s="339" t="s">
         <v>18</v>
       </c>
-      <c r="AA44" s="332"/>
-      <c r="AB44" s="332"/>
-      <c r="AC44" s="332" t="s">
+      <c r="AA44" s="339"/>
+      <c r="AB44" s="339"/>
+      <c r="AC44" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="AD44" s="332"/>
-      <c r="AE44" s="332"/>
-      <c r="AF44" s="332" t="s">
+      <c r="AD44" s="339"/>
+      <c r="AE44" s="339"/>
+      <c r="AF44" s="339" t="s">
         <v>20</v>
       </c>
-      <c r="AG44" s="332"/>
-      <c r="AH44" s="332"/>
-      <c r="AI44" s="332" t="s">
+      <c r="AG44" s="339"/>
+      <c r="AH44" s="339"/>
+      <c r="AI44" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="AJ44" s="332"/>
-      <c r="AK44" s="333"/>
-      <c r="AL44" s="339" t="s">
+      <c r="AJ44" s="339"/>
+      <c r="AK44" s="340"/>
+      <c r="AL44" s="341" t="s">
         <v>45</v>
       </c>
-      <c r="AM44" s="332"/>
-      <c r="AN44" s="332"/>
-      <c r="AO44" s="332" t="s">
+      <c r="AM44" s="339"/>
+      <c r="AN44" s="339"/>
+      <c r="AO44" s="339" t="s">
         <v>17</v>
       </c>
-      <c r="AP44" s="332"/>
-      <c r="AQ44" s="332"/>
-      <c r="AR44" s="332" t="s">
+      <c r="AP44" s="339"/>
+      <c r="AQ44" s="339"/>
+      <c r="AR44" s="339" t="s">
         <v>18</v>
       </c>
-      <c r="AS44" s="332"/>
-      <c r="AT44" s="332"/>
-      <c r="AU44" s="332" t="s">
+      <c r="AS44" s="339"/>
+      <c r="AT44" s="339"/>
+      <c r="AU44" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="AV44" s="332"/>
-      <c r="AW44" s="332"/>
-      <c r="AX44" s="332" t="s">
+      <c r="AV44" s="339"/>
+      <c r="AW44" s="339"/>
+      <c r="AX44" s="339" t="s">
         <v>20</v>
       </c>
-      <c r="AY44" s="332"/>
-      <c r="AZ44" s="332"/>
-      <c r="BA44" s="332" t="s">
+      <c r="AY44" s="339"/>
+      <c r="AZ44" s="339"/>
+      <c r="BA44" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="BB44" s="332"/>
-      <c r="BC44" s="333"/>
+      <c r="BB44" s="339"/>
+      <c r="BC44" s="340"/>
     </row>
     <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
@@ -6604,61 +6685,61 @@
     </row>
     <row r="64" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="334" t="s">
+      <c r="B64" s="328" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="334"/>
-      <c r="D64" s="334"/>
-      <c r="E64" s="334"/>
-      <c r="F64" s="334"/>
-      <c r="G64" s="334"/>
-      <c r="H64" s="334"/>
-      <c r="I64" s="334"/>
-      <c r="J64" s="334"/>
-      <c r="K64" s="324"/>
-      <c r="L64" s="334" t="s">
+      <c r="C64" s="328"/>
+      <c r="D64" s="328"/>
+      <c r="E64" s="328"/>
+      <c r="F64" s="328"/>
+      <c r="G64" s="328"/>
+      <c r="H64" s="328"/>
+      <c r="I64" s="328"/>
+      <c r="J64" s="328"/>
+      <c r="K64" s="329"/>
+      <c r="L64" s="328" t="s">
         <v>83</v>
       </c>
-      <c r="M64" s="334"/>
-      <c r="N64" s="334"/>
-      <c r="O64" s="334"/>
-      <c r="P64" s="334"/>
-      <c r="Q64" s="334"/>
-      <c r="R64" s="334"/>
-      <c r="S64" s="334"/>
-      <c r="T64" s="334"/>
-      <c r="U64" s="324"/>
+      <c r="M64" s="328"/>
+      <c r="N64" s="328"/>
+      <c r="O64" s="328"/>
+      <c r="P64" s="328"/>
+      <c r="Q64" s="328"/>
+      <c r="R64" s="328"/>
+      <c r="S64" s="328"/>
+      <c r="T64" s="328"/>
+      <c r="U64" s="329"/>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="B65" s="338" t="s">
+      <c r="B65" s="327" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="334"/>
-      <c r="D65" s="334"/>
-      <c r="E65" s="334"/>
-      <c r="F65" s="324"/>
-      <c r="G65" s="334" t="s">
+      <c r="C65" s="328"/>
+      <c r="D65" s="328"/>
+      <c r="E65" s="328"/>
+      <c r="F65" s="329"/>
+      <c r="G65" s="328" t="s">
         <v>81</v>
       </c>
-      <c r="H65" s="334"/>
-      <c r="I65" s="334"/>
-      <c r="J65" s="334"/>
-      <c r="K65" s="324"/>
-      <c r="L65" s="334" t="s">
+      <c r="H65" s="328"/>
+      <c r="I65" s="328"/>
+      <c r="J65" s="328"/>
+      <c r="K65" s="329"/>
+      <c r="L65" s="328" t="s">
         <v>80</v>
       </c>
-      <c r="M65" s="334"/>
-      <c r="N65" s="334"/>
-      <c r="O65" s="334"/>
-      <c r="P65" s="324"/>
-      <c r="Q65" s="334" t="s">
+      <c r="M65" s="328"/>
+      <c r="N65" s="328"/>
+      <c r="O65" s="328"/>
+      <c r="P65" s="329"/>
+      <c r="Q65" s="328" t="s">
         <v>81</v>
       </c>
-      <c r="R65" s="334"/>
-      <c r="S65" s="334"/>
-      <c r="T65" s="334"/>
-      <c r="U65" s="324"/>
+      <c r="R65" s="328"/>
+      <c r="S65" s="328"/>
+      <c r="T65" s="328"/>
+      <c r="U65" s="329"/>
     </row>
     <row r="66" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
@@ -6787,19 +6868,19 @@
       <c r="U67" s="137">
         <v>0.08</v>
       </c>
-      <c r="X67" s="326" t="s">
+      <c r="X67" s="330" t="s">
         <v>102</v>
       </c>
-      <c r="Y67" s="326"/>
-      <c r="Z67" s="326"/>
-      <c r="AA67" s="326"/>
-      <c r="AB67" s="326"/>
-      <c r="AC67" s="326"/>
-      <c r="AD67" s="326"/>
-      <c r="AE67" s="326"/>
-      <c r="AF67" s="326"/>
-      <c r="AG67" s="326"/>
-      <c r="AH67" s="326"/>
+      <c r="Y67" s="330"/>
+      <c r="Z67" s="330"/>
+      <c r="AA67" s="330"/>
+      <c r="AB67" s="330"/>
+      <c r="AC67" s="330"/>
+      <c r="AD67" s="330"/>
+      <c r="AE67" s="330"/>
+      <c r="AF67" s="330"/>
+      <c r="AG67" s="330"/>
+      <c r="AH67" s="330"/>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68" s="127" t="s">
@@ -6865,20 +6946,20 @@
       <c r="U68" s="5">
         <v>0.05</v>
       </c>
-      <c r="Y68" s="327" t="s">
+      <c r="Y68" s="332" t="s">
         <v>40</v>
       </c>
-      <c r="Z68" s="328"/>
-      <c r="AA68" s="328"/>
-      <c r="AB68" s="328"/>
-      <c r="AC68" s="329"/>
-      <c r="AD68" s="328" t="s">
+      <c r="Z68" s="333"/>
+      <c r="AA68" s="333"/>
+      <c r="AB68" s="333"/>
+      <c r="AC68" s="334"/>
+      <c r="AD68" s="333" t="s">
         <v>39</v>
       </c>
-      <c r="AE68" s="328"/>
-      <c r="AF68" s="328"/>
-      <c r="AG68" s="328"/>
-      <c r="AH68" s="329"/>
+      <c r="AE68" s="333"/>
+      <c r="AF68" s="333"/>
+      <c r="AG68" s="333"/>
+      <c r="AH68" s="334"/>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="127" t="s">
@@ -7007,10 +7088,10 @@
       <c r="S70" s="132"/>
       <c r="T70" s="132"/>
       <c r="U70" s="133"/>
-      <c r="W70" s="326" t="s">
+      <c r="W70" s="330" t="s">
         <v>25</v>
       </c>
-      <c r="X70" s="330"/>
+      <c r="X70" s="331"/>
       <c r="Y70" s="53"/>
       <c r="Z70" s="14"/>
       <c r="AA70" s="14"/>
@@ -7086,10 +7167,10 @@
       <c r="U71" s="137">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W71" s="326" t="s">
+      <c r="W71" s="330" t="s">
         <v>26</v>
       </c>
-      <c r="X71" s="330"/>
+      <c r="X71" s="331"/>
       <c r="Y71" s="156">
         <v>0.14179</v>
       </c>
@@ -7185,10 +7266,10 @@
       <c r="U72" s="148">
         <v>0.03</v>
       </c>
-      <c r="W72" s="326" t="s">
+      <c r="W72" s="330" t="s">
         <v>27</v>
       </c>
-      <c r="X72" s="330"/>
+      <c r="X72" s="331"/>
       <c r="Y72" s="156">
         <v>0.125</v>
       </c>
@@ -7284,10 +7365,10 @@
       <c r="U73" s="137">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W73" s="326" t="s">
+      <c r="W73" s="330" t="s">
         <v>28</v>
       </c>
-      <c r="X73" s="330"/>
+      <c r="X73" s="331"/>
       <c r="Y73" s="156">
         <v>0.3</v>
       </c>
@@ -7383,10 +7464,10 @@
       <c r="U74" s="140">
         <v>6.7831876028940266E-2</v>
       </c>
-      <c r="W74" s="326" t="s">
+      <c r="W74" s="330" t="s">
         <v>29</v>
       </c>
-      <c r="X74" s="330"/>
+      <c r="X74" s="331"/>
       <c r="Y74" s="156">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -7482,10 +7563,10 @@
       <c r="U75" s="137">
         <v>0.06</v>
       </c>
-      <c r="W75" s="326" t="s">
+      <c r="W75" s="330" t="s">
         <v>36</v>
       </c>
-      <c r="X75" s="330"/>
+      <c r="X75" s="331"/>
       <c r="Y75" s="156">
         <v>0.255</v>
       </c>
@@ -7581,10 +7662,10 @@
       <c r="U76" s="137">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W76" s="326" t="s">
+      <c r="W76" s="330" t="s">
         <v>38</v>
       </c>
-      <c r="X76" s="330"/>
+      <c r="X76" s="331"/>
       <c r="Y76" s="167">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -7680,10 +7761,10 @@
       <c r="U77" s="199">
         <v>0.01</v>
       </c>
-      <c r="W77" s="326" t="s">
+      <c r="W77" s="330" t="s">
         <v>41</v>
       </c>
-      <c r="X77" s="330"/>
+      <c r="X77" s="331"/>
       <c r="Y77" s="162">
         <v>7.5743000000000005E-2</v>
       </c>
@@ -8106,34 +8187,34 @@
       </c>
     </row>
     <row r="84" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="344" t="s">
+      <c r="B84" s="324" t="s">
         <v>80</v>
       </c>
-      <c r="C84" s="345"/>
-      <c r="D84" s="345"/>
-      <c r="E84" s="345"/>
-      <c r="F84" s="346"/>
-      <c r="G84" s="345" t="s">
+      <c r="C84" s="325"/>
+      <c r="D84" s="325"/>
+      <c r="E84" s="325"/>
+      <c r="F84" s="326"/>
+      <c r="G84" s="325" t="s">
         <v>81</v>
       </c>
-      <c r="H84" s="345"/>
-      <c r="I84" s="345"/>
-      <c r="J84" s="345"/>
-      <c r="K84" s="346"/>
-      <c r="L84" s="345" t="s">
+      <c r="H84" s="325"/>
+      <c r="I84" s="325"/>
+      <c r="J84" s="325"/>
+      <c r="K84" s="326"/>
+      <c r="L84" s="325" t="s">
         <v>80</v>
       </c>
-      <c r="M84" s="345"/>
-      <c r="N84" s="345"/>
-      <c r="O84" s="345"/>
-      <c r="P84" s="346"/>
-      <c r="Q84" s="345" t="s">
+      <c r="M84" s="325"/>
+      <c r="N84" s="325"/>
+      <c r="O84" s="325"/>
+      <c r="P84" s="326"/>
+      <c r="Q84" s="325" t="s">
         <v>81</v>
       </c>
-      <c r="R84" s="345"/>
-      <c r="S84" s="345"/>
-      <c r="T84" s="345"/>
-      <c r="U84" s="346"/>
+      <c r="R84" s="325"/>
+      <c r="S84" s="325"/>
+      <c r="T84" s="325"/>
+      <c r="U84" s="326"/>
     </row>
     <row r="85" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" s="174" t="s">
@@ -8196,19 +8277,19 @@
       <c r="U85" s="176" t="s">
         <v>30</v>
       </c>
-      <c r="X85" s="326" t="s">
+      <c r="X85" s="330" t="s">
         <v>103</v>
       </c>
-      <c r="Y85" s="326"/>
-      <c r="Z85" s="326"/>
-      <c r="AA85" s="326"/>
-      <c r="AB85" s="326"/>
-      <c r="AC85" s="326"/>
-      <c r="AD85" s="326"/>
-      <c r="AE85" s="326"/>
-      <c r="AF85" s="326"/>
-      <c r="AG85" s="326"/>
-      <c r="AH85" s="326"/>
+      <c r="Y85" s="330"/>
+      <c r="Z85" s="330"/>
+      <c r="AA85" s="330"/>
+      <c r="AB85" s="330"/>
+      <c r="AC85" s="330"/>
+      <c r="AD85" s="330"/>
+      <c r="AE85" s="330"/>
+      <c r="AF85" s="330"/>
+      <c r="AG85" s="330"/>
+      <c r="AH85" s="330"/>
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" s="178" t="s">
@@ -8274,20 +8355,20 @@
       <c r="U86" s="140">
         <v>9.7044040453526839E-2</v>
       </c>
-      <c r="Y86" s="327" t="s">
+      <c r="Y86" s="332" t="s">
         <v>40</v>
       </c>
-      <c r="Z86" s="328"/>
-      <c r="AA86" s="328"/>
-      <c r="AB86" s="328"/>
-      <c r="AC86" s="329"/>
-      <c r="AD86" s="328" t="s">
+      <c r="Z86" s="333"/>
+      <c r="AA86" s="333"/>
+      <c r="AB86" s="333"/>
+      <c r="AC86" s="334"/>
+      <c r="AD86" s="333" t="s">
         <v>39</v>
       </c>
-      <c r="AE86" s="328"/>
-      <c r="AF86" s="328"/>
-      <c r="AG86" s="328"/>
-      <c r="AH86" s="329"/>
+      <c r="AE86" s="333"/>
+      <c r="AF86" s="333"/>
+      <c r="AG86" s="333"/>
+      <c r="AH86" s="334"/>
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" s="127" t="s">
@@ -8448,10 +8529,10 @@
       <c r="U88" s="148">
         <v>0.06</v>
       </c>
-      <c r="W88" s="326" t="s">
+      <c r="W88" s="330" t="s">
         <v>25</v>
       </c>
-      <c r="X88" s="330"/>
+      <c r="X88" s="331"/>
       <c r="Y88" s="53"/>
       <c r="Z88" s="14"/>
       <c r="AA88" s="14"/>
@@ -8527,10 +8608,10 @@
       <c r="U89" s="137">
         <v>0.09</v>
       </c>
-      <c r="W89" s="326" t="s">
+      <c r="W89" s="330" t="s">
         <v>26</v>
       </c>
-      <c r="X89" s="330"/>
+      <c r="X89" s="331"/>
       <c r="Y89" s="156">
         <v>0.17732999999999999</v>
       </c>
@@ -8626,10 +8707,10 @@
       <c r="U90" s="148">
         <v>0.05</v>
       </c>
-      <c r="W90" s="326" t="s">
+      <c r="W90" s="330" t="s">
         <v>27</v>
       </c>
-      <c r="X90" s="330"/>
+      <c r="X90" s="331"/>
       <c r="Y90" s="156">
         <v>0.16</v>
       </c>
@@ -8725,10 +8806,10 @@
       <c r="U91" s="143">
         <v>5.2339410766781939E-2</v>
       </c>
-      <c r="W91" s="326" t="s">
+      <c r="W91" s="330" t="s">
         <v>28</v>
       </c>
-      <c r="X91" s="330"/>
+      <c r="X91" s="331"/>
       <c r="Y91" s="156">
         <v>0.28000000000000003</v>
       </c>
@@ -8824,10 +8905,10 @@
       <c r="U92" s="143">
         <v>4.5787429941166059E-2</v>
       </c>
-      <c r="W92" s="326" t="s">
+      <c r="W92" s="330" t="s">
         <v>29</v>
       </c>
-      <c r="X92" s="330"/>
+      <c r="X92" s="331"/>
       <c r="Y92" s="156">
         <v>0.11</v>
       </c>
@@ -8923,10 +9004,10 @@
       <c r="U93" s="140">
         <v>6.72497190179734E-2</v>
       </c>
-      <c r="W93" s="326" t="s">
+      <c r="W93" s="330" t="s">
         <v>36</v>
       </c>
-      <c r="X93" s="330"/>
+      <c r="X93" s="331"/>
       <c r="Y93" s="156">
         <v>0.17</v>
       </c>
@@ -9022,10 +9103,10 @@
       <c r="U94" s="140">
         <v>0.10088850483912387</v>
       </c>
-      <c r="W94" s="326" t="s">
+      <c r="W94" s="330" t="s">
         <v>38</v>
       </c>
-      <c r="X94" s="330"/>
+      <c r="X94" s="331"/>
       <c r="Y94" s="167">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -9121,10 +9202,10 @@
       <c r="U95" s="148">
         <v>0.05</v>
       </c>
-      <c r="W95" s="326" t="s">
+      <c r="W95" s="330" t="s">
         <v>41</v>
       </c>
-      <c r="X95" s="330"/>
+      <c r="X95" s="331"/>
       <c r="Y95" s="162">
         <v>5.5608999999999999E-2</v>
       </c>
@@ -9287,42 +9368,42 @@
       </c>
     </row>
     <row r="98" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="324"/>
-      <c r="B98" s="338" t="s">
+      <c r="A98" s="329"/>
+      <c r="B98" s="327" t="s">
         <v>80</v>
       </c>
-      <c r="C98" s="334"/>
-      <c r="D98" s="334"/>
-      <c r="E98" s="334"/>
-      <c r="F98" s="334"/>
-      <c r="G98" s="324"/>
-      <c r="H98" s="334" t="s">
+      <c r="C98" s="328"/>
+      <c r="D98" s="328"/>
+      <c r="E98" s="328"/>
+      <c r="F98" s="328"/>
+      <c r="G98" s="329"/>
+      <c r="H98" s="328" t="s">
         <v>81</v>
       </c>
-      <c r="I98" s="334"/>
-      <c r="J98" s="334"/>
-      <c r="K98" s="334"/>
-      <c r="L98" s="334"/>
-      <c r="M98" s="324"/>
-      <c r="N98" s="334" t="s">
+      <c r="I98" s="328"/>
+      <c r="J98" s="328"/>
+      <c r="K98" s="328"/>
+      <c r="L98" s="328"/>
+      <c r="M98" s="329"/>
+      <c r="N98" s="328" t="s">
         <v>80</v>
       </c>
-      <c r="O98" s="334"/>
-      <c r="P98" s="334"/>
-      <c r="Q98" s="334"/>
-      <c r="R98" s="334"/>
-      <c r="S98" s="324"/>
-      <c r="T98" s="334" t="s">
+      <c r="O98" s="328"/>
+      <c r="P98" s="328"/>
+      <c r="Q98" s="328"/>
+      <c r="R98" s="328"/>
+      <c r="S98" s="329"/>
+      <c r="T98" s="328" t="s">
         <v>81</v>
       </c>
-      <c r="U98" s="334"/>
-      <c r="V98" s="334"/>
-      <c r="W98" s="334"/>
-      <c r="X98" s="334"/>
-      <c r="Y98" s="324"/>
+      <c r="U98" s="328"/>
+      <c r="V98" s="328"/>
+      <c r="W98" s="328"/>
+      <c r="X98" s="328"/>
+      <c r="Y98" s="329"/>
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A99" s="325"/>
+      <c r="A99" s="338"/>
       <c r="B99" s="1" t="s">
         <v>100</v>
       </c>
@@ -9629,19 +9710,56 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="G84:K84"/>
-    <mergeCell ref="L84:P84"/>
-    <mergeCell ref="Q84:U84"/>
-    <mergeCell ref="B98:G98"/>
-    <mergeCell ref="H98:M98"/>
-    <mergeCell ref="N98:S98"/>
-    <mergeCell ref="T98:Y98"/>
-    <mergeCell ref="W73:X73"/>
-    <mergeCell ref="W74:X74"/>
-    <mergeCell ref="W75:X75"/>
-    <mergeCell ref="W76:X76"/>
-    <mergeCell ref="W77:X77"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="X85:AH85"/>
+    <mergeCell ref="Y86:AC86"/>
+    <mergeCell ref="AD86:AH86"/>
+    <mergeCell ref="W88:X88"/>
+    <mergeCell ref="W89:X89"/>
+    <mergeCell ref="W90:X90"/>
+    <mergeCell ref="W91:X91"/>
+    <mergeCell ref="W92:X92"/>
+    <mergeCell ref="W93:X93"/>
+    <mergeCell ref="W94:X94"/>
+    <mergeCell ref="W95:X95"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="S22:AF22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AD23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="AL43:AZ43"/>
+    <mergeCell ref="AU44:AW44"/>
+    <mergeCell ref="AX44:AZ44"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="Z44:AB44"/>
+    <mergeCell ref="AC44:AE44"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="G65:K65"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="BA44:BC44"/>
+    <mergeCell ref="AF44:AH44"/>
+    <mergeCell ref="AI44:AK44"/>
+    <mergeCell ref="AL44:AN44"/>
+    <mergeCell ref="AO44:AQ44"/>
+    <mergeCell ref="AR44:AT44"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="L65:P65"/>
+    <mergeCell ref="Q65:U65"/>
     <mergeCell ref="S1:AC1"/>
     <mergeCell ref="X67:AH67"/>
     <mergeCell ref="Y68:AC68"/>
@@ -9658,56 +9776,19 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="B43:P43"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="G65:K65"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="BA44:BC44"/>
-    <mergeCell ref="AF44:AH44"/>
-    <mergeCell ref="AI44:AK44"/>
-    <mergeCell ref="AL44:AN44"/>
-    <mergeCell ref="AO44:AQ44"/>
-    <mergeCell ref="AR44:AT44"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="L65:P65"/>
-    <mergeCell ref="Q65:U65"/>
-    <mergeCell ref="AL43:AZ43"/>
-    <mergeCell ref="AU44:AW44"/>
-    <mergeCell ref="AX44:AZ44"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="Z44:AB44"/>
-    <mergeCell ref="AC44:AE44"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="S22:AF22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AD23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="X85:AH85"/>
-    <mergeCell ref="Y86:AC86"/>
-    <mergeCell ref="AD86:AH86"/>
-    <mergeCell ref="W88:X88"/>
-    <mergeCell ref="W89:X89"/>
-    <mergeCell ref="W90:X90"/>
-    <mergeCell ref="W91:X91"/>
-    <mergeCell ref="W92:X92"/>
-    <mergeCell ref="W93:X93"/>
-    <mergeCell ref="W94:X94"/>
-    <mergeCell ref="W95:X95"/>
+    <mergeCell ref="W73:X73"/>
+    <mergeCell ref="W74:X74"/>
+    <mergeCell ref="W75:X75"/>
+    <mergeCell ref="W76:X76"/>
+    <mergeCell ref="W77:X77"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="G84:K84"/>
+    <mergeCell ref="L84:P84"/>
+    <mergeCell ref="Q84:U84"/>
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="H98:M98"/>
+    <mergeCell ref="N98:S98"/>
+    <mergeCell ref="T98:Y98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9721,7 +9802,7 @@
   </sheetPr>
   <dimension ref="A1:AY46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
       <selection pane="topRight" activeCell="AG36" sqref="AG36:AK36"/>
@@ -9758,48 +9839,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="354" t="s">
+      <c r="A1" s="367" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="368"/>
-      <c r="C1" s="368"/>
-      <c r="D1" s="368"/>
-      <c r="E1" s="368"/>
-      <c r="F1" s="368"/>
-      <c r="G1" s="368"/>
-      <c r="H1" s="368"/>
-      <c r="I1" s="368"/>
-      <c r="J1" s="368"/>
-      <c r="K1" s="369"/>
+      <c r="B1" s="360"/>
+      <c r="C1" s="360"/>
+      <c r="D1" s="360"/>
+      <c r="E1" s="360"/>
+      <c r="F1" s="360"/>
+      <c r="G1" s="360"/>
+      <c r="H1" s="360"/>
+      <c r="I1" s="360"/>
+      <c r="J1" s="360"/>
+      <c r="K1" s="361"/>
       <c r="L1" s="64"/>
-      <c r="M1" s="354" t="s">
+      <c r="M1" s="367" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="355"/>
-      <c r="O1" s="355"/>
-      <c r="P1" s="355"/>
-      <c r="Q1" s="355"/>
-      <c r="R1" s="355"/>
-      <c r="S1" s="355"/>
-      <c r="T1" s="355"/>
-      <c r="U1" s="355"/>
-      <c r="V1" s="355"/>
-      <c r="W1" s="355"/>
-      <c r="X1" s="355"/>
-      <c r="Y1" s="355"/>
-      <c r="Z1" s="355"/>
-      <c r="AA1" s="355"/>
-      <c r="AB1" s="355"/>
-      <c r="AC1" s="355"/>
-      <c r="AD1" s="355"/>
-      <c r="AE1" s="355"/>
-      <c r="AF1" s="355"/>
-      <c r="AG1" s="355"/>
-      <c r="AH1" s="355"/>
-      <c r="AI1" s="355"/>
-      <c r="AJ1" s="355"/>
-      <c r="AK1" s="355"/>
-      <c r="AL1" s="356"/>
+      <c r="N1" s="383"/>
+      <c r="O1" s="383"/>
+      <c r="P1" s="383"/>
+      <c r="Q1" s="383"/>
+      <c r="R1" s="383"/>
+      <c r="S1" s="383"/>
+      <c r="T1" s="383"/>
+      <c r="U1" s="383"/>
+      <c r="V1" s="383"/>
+      <c r="W1" s="383"/>
+      <c r="X1" s="383"/>
+      <c r="Y1" s="383"/>
+      <c r="Z1" s="383"/>
+      <c r="AA1" s="383"/>
+      <c r="AB1" s="383"/>
+      <c r="AC1" s="383"/>
+      <c r="AD1" s="383"/>
+      <c r="AE1" s="383"/>
+      <c r="AF1" s="383"/>
+      <c r="AG1" s="383"/>
+      <c r="AH1" s="383"/>
+      <c r="AI1" s="383"/>
+      <c r="AJ1" s="383"/>
+      <c r="AK1" s="383"/>
+      <c r="AL1" s="384"/>
       <c r="AM1" s="70"/>
       <c r="AN1" s="70"/>
       <c r="AO1" s="70"/>
@@ -9815,44 +9896,44 @@
       <c r="AY1" s="71"/>
     </row>
     <row r="2" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="357"/>
-      <c r="B2" s="370"/>
-      <c r="C2" s="370"/>
-      <c r="D2" s="370"/>
-      <c r="E2" s="370"/>
-      <c r="F2" s="370"/>
-      <c r="G2" s="370"/>
-      <c r="H2" s="370"/>
-      <c r="I2" s="370"/>
-      <c r="J2" s="370"/>
-      <c r="K2" s="371"/>
+      <c r="A2" s="368"/>
+      <c r="B2" s="369"/>
+      <c r="C2" s="369"/>
+      <c r="D2" s="369"/>
+      <c r="E2" s="369"/>
+      <c r="F2" s="369"/>
+      <c r="G2" s="369"/>
+      <c r="H2" s="369"/>
+      <c r="I2" s="369"/>
+      <c r="J2" s="369"/>
+      <c r="K2" s="370"/>
       <c r="L2" s="73"/>
-      <c r="M2" s="357"/>
-      <c r="N2" s="358"/>
-      <c r="O2" s="358"/>
-      <c r="P2" s="358"/>
-      <c r="Q2" s="358"/>
-      <c r="R2" s="358"/>
-      <c r="S2" s="358"/>
-      <c r="T2" s="358"/>
-      <c r="U2" s="358"/>
-      <c r="V2" s="358"/>
-      <c r="W2" s="358"/>
-      <c r="X2" s="358"/>
-      <c r="Y2" s="358"/>
-      <c r="Z2" s="358"/>
-      <c r="AA2" s="358"/>
-      <c r="AB2" s="358"/>
-      <c r="AC2" s="358"/>
-      <c r="AD2" s="358"/>
-      <c r="AE2" s="358"/>
-      <c r="AF2" s="358"/>
-      <c r="AG2" s="358"/>
-      <c r="AH2" s="358"/>
-      <c r="AI2" s="358"/>
-      <c r="AJ2" s="358"/>
-      <c r="AK2" s="358"/>
-      <c r="AL2" s="359"/>
+      <c r="M2" s="368"/>
+      <c r="N2" s="385"/>
+      <c r="O2" s="385"/>
+      <c r="P2" s="385"/>
+      <c r="Q2" s="385"/>
+      <c r="R2" s="385"/>
+      <c r="S2" s="385"/>
+      <c r="T2" s="385"/>
+      <c r="U2" s="385"/>
+      <c r="V2" s="385"/>
+      <c r="W2" s="385"/>
+      <c r="X2" s="385"/>
+      <c r="Y2" s="385"/>
+      <c r="Z2" s="385"/>
+      <c r="AA2" s="385"/>
+      <c r="AB2" s="385"/>
+      <c r="AC2" s="385"/>
+      <c r="AD2" s="385"/>
+      <c r="AE2" s="385"/>
+      <c r="AF2" s="385"/>
+      <c r="AG2" s="385"/>
+      <c r="AH2" s="385"/>
+      <c r="AI2" s="385"/>
+      <c r="AJ2" s="385"/>
+      <c r="AK2" s="385"/>
+      <c r="AL2" s="386"/>
       <c r="AM2" s="65"/>
       <c r="AN2" s="65"/>
       <c r="AO2" s="65"/>
@@ -9868,7 +9949,7 @@
       <c r="AY2" s="72"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3" s="378"/>
+      <c r="A3" s="377"/>
       <c r="B3" s="92" t="s">
         <v>67</v>
       </c>
@@ -9887,57 +9968,57 @@
       <c r="G3" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="382" t="s">
+      <c r="H3" s="380" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="367" t="s">
+      <c r="I3" s="364" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="367" t="s">
+      <c r="J3" s="364" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="351" t="s">
+      <c r="K3" s="365" t="s">
         <v>61</v>
       </c>
       <c r="L3" s="76"/>
-      <c r="M3" s="372"/>
-      <c r="N3" s="373"/>
-      <c r="O3" s="366" t="s">
+      <c r="M3" s="371"/>
+      <c r="N3" s="372"/>
+      <c r="O3" s="359" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="367"/>
-      <c r="Q3" s="367"/>
-      <c r="R3" s="351"/>
-      <c r="S3" s="367" t="s">
+      <c r="P3" s="364"/>
+      <c r="Q3" s="364"/>
+      <c r="R3" s="365"/>
+      <c r="S3" s="364" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="367"/>
-      <c r="U3" s="367"/>
-      <c r="V3" s="351"/>
-      <c r="W3" s="349" t="s">
+      <c r="T3" s="364"/>
+      <c r="U3" s="364"/>
+      <c r="V3" s="365"/>
+      <c r="W3" s="389" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="349"/>
-      <c r="Y3" s="349"/>
-      <c r="Z3" s="350"/>
-      <c r="AA3" s="349" t="s">
+      <c r="X3" s="389"/>
+      <c r="Y3" s="389"/>
+      <c r="Z3" s="390"/>
+      <c r="AA3" s="389" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="349"/>
-      <c r="AC3" s="349"/>
-      <c r="AD3" s="350"/>
-      <c r="AE3" s="349" t="s">
+      <c r="AB3" s="389"/>
+      <c r="AC3" s="389"/>
+      <c r="AD3" s="390"/>
+      <c r="AE3" s="389" t="s">
         <v>20</v>
       </c>
-      <c r="AF3" s="349"/>
-      <c r="AG3" s="349"/>
-      <c r="AH3" s="350"/>
-      <c r="AI3" s="349" t="s">
+      <c r="AF3" s="389"/>
+      <c r="AG3" s="389"/>
+      <c r="AH3" s="390"/>
+      <c r="AI3" s="389" t="s">
         <v>21</v>
       </c>
-      <c r="AJ3" s="349"/>
-      <c r="AK3" s="349"/>
-      <c r="AL3" s="350"/>
+      <c r="AJ3" s="389"/>
+      <c r="AK3" s="389"/>
+      <c r="AL3" s="390"/>
       <c r="AM3" s="67"/>
       <c r="AN3" s="67"/>
       <c r="AO3" s="67"/>
@@ -9953,80 +10034,80 @@
       <c r="AY3" s="67"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4" s="379"/>
-      <c r="B4" s="360" t="s">
+      <c r="A4" s="378"/>
+      <c r="B4" s="347" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="362" t="s">
+      <c r="C4" s="348" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="362" t="s">
+      <c r="D4" s="348" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="362" t="s">
+      <c r="E4" s="348" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="362" t="s">
+      <c r="F4" s="348" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="364" t="s">
+      <c r="G4" s="387" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="383"/>
-      <c r="I4" s="362"/>
-      <c r="J4" s="362"/>
-      <c r="K4" s="352"/>
+      <c r="H4" s="381"/>
+      <c r="I4" s="348"/>
+      <c r="J4" s="348"/>
+      <c r="K4" s="349"/>
       <c r="L4" s="76"/>
-      <c r="M4" s="374"/>
-      <c r="N4" s="375"/>
-      <c r="O4" s="360" t="s">
+      <c r="M4" s="373"/>
+      <c r="N4" s="374"/>
+      <c r="O4" s="347" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="362"/>
-      <c r="Q4" s="362" t="s">
+      <c r="P4" s="348"/>
+      <c r="Q4" s="348" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="352"/>
-      <c r="S4" s="362" t="s">
+      <c r="R4" s="349"/>
+      <c r="S4" s="348" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="362"/>
-      <c r="U4" s="362" t="s">
+      <c r="T4" s="348"/>
+      <c r="U4" s="348" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="352"/>
-      <c r="W4" s="347" t="s">
+      <c r="V4" s="349"/>
+      <c r="W4" s="391" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="347"/>
-      <c r="Y4" s="347" t="s">
+      <c r="X4" s="391"/>
+      <c r="Y4" s="391" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="348"/>
-      <c r="AA4" s="347" t="s">
+      <c r="Z4" s="392"/>
+      <c r="AA4" s="391" t="s">
         <v>65</v>
       </c>
-      <c r="AB4" s="347"/>
-      <c r="AC4" s="347" t="s">
+      <c r="AB4" s="391"/>
+      <c r="AC4" s="391" t="s">
         <v>66</v>
       </c>
-      <c r="AD4" s="348"/>
-      <c r="AE4" s="347" t="s">
+      <c r="AD4" s="392"/>
+      <c r="AE4" s="391" t="s">
         <v>65</v>
       </c>
-      <c r="AF4" s="347"/>
-      <c r="AG4" s="347" t="s">
+      <c r="AF4" s="391"/>
+      <c r="AG4" s="391" t="s">
         <v>66</v>
       </c>
-      <c r="AH4" s="348"/>
-      <c r="AI4" s="347" t="s">
+      <c r="AH4" s="392"/>
+      <c r="AI4" s="391" t="s">
         <v>65</v>
       </c>
-      <c r="AJ4" s="347"/>
-      <c r="AK4" s="347" t="s">
+      <c r="AJ4" s="391"/>
+      <c r="AK4" s="391" t="s">
         <v>66</v>
       </c>
-      <c r="AL4" s="348"/>
+      <c r="AL4" s="392"/>
       <c r="AM4" s="67"/>
       <c r="AN4" s="67"/>
       <c r="AO4" s="67"/>
@@ -10042,20 +10123,20 @@
       <c r="AY4" s="67"/>
     </row>
     <row r="5" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="380"/>
-      <c r="B5" s="361"/>
-      <c r="C5" s="363"/>
-      <c r="D5" s="363"/>
-      <c r="E5" s="363"/>
-      <c r="F5" s="363"/>
-      <c r="G5" s="365"/>
-      <c r="H5" s="384"/>
-      <c r="I5" s="363"/>
-      <c r="J5" s="363"/>
-      <c r="K5" s="353"/>
+      <c r="A5" s="379"/>
+      <c r="B5" s="353"/>
+      <c r="C5" s="354"/>
+      <c r="D5" s="354"/>
+      <c r="E5" s="354"/>
+      <c r="F5" s="354"/>
+      <c r="G5" s="388"/>
+      <c r="H5" s="382"/>
+      <c r="I5" s="354"/>
+      <c r="J5" s="354"/>
+      <c r="K5" s="355"/>
       <c r="L5" s="77"/>
-      <c r="M5" s="376"/>
-      <c r="N5" s="377"/>
+      <c r="M5" s="375"/>
+      <c r="N5" s="376"/>
       <c r="O5" s="94" t="s">
         <v>64</v>
       </c>
@@ -11476,47 +11557,47 @@
     </row>
     <row r="24" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="354" t="s">
+      <c r="A25" s="367" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="368"/>
-      <c r="C25" s="368"/>
-      <c r="D25" s="368"/>
-      <c r="E25" s="368"/>
-      <c r="F25" s="368"/>
-      <c r="G25" s="368"/>
-      <c r="H25" s="368"/>
-      <c r="I25" s="368"/>
-      <c r="J25" s="368"/>
-      <c r="K25" s="368"/>
-      <c r="L25" s="368"/>
-      <c r="M25" s="368"/>
-      <c r="N25" s="368"/>
-      <c r="O25" s="368"/>
-      <c r="P25" s="368"/>
-      <c r="Q25" s="368"/>
-      <c r="R25" s="368"/>
-      <c r="S25" s="368"/>
-      <c r="T25" s="368"/>
-      <c r="U25" s="369"/>
-      <c r="X25" s="366"/>
-      <c r="Y25" s="368" t="s">
+      <c r="B25" s="360"/>
+      <c r="C25" s="360"/>
+      <c r="D25" s="360"/>
+      <c r="E25" s="360"/>
+      <c r="F25" s="360"/>
+      <c r="G25" s="360"/>
+      <c r="H25" s="360"/>
+      <c r="I25" s="360"/>
+      <c r="J25" s="360"/>
+      <c r="K25" s="360"/>
+      <c r="L25" s="360"/>
+      <c r="M25" s="360"/>
+      <c r="N25" s="360"/>
+      <c r="O25" s="360"/>
+      <c r="P25" s="360"/>
+      <c r="Q25" s="360"/>
+      <c r="R25" s="360"/>
+      <c r="S25" s="360"/>
+      <c r="T25" s="360"/>
+      <c r="U25" s="361"/>
+      <c r="X25" s="359"/>
+      <c r="Y25" s="360" t="s">
         <v>180</v>
       </c>
-      <c r="Z25" s="368"/>
-      <c r="AA25" s="368"/>
-      <c r="AB25" s="368"/>
-      <c r="AC25" s="369"/>
+      <c r="Z25" s="360"/>
+      <c r="AA25" s="360"/>
+      <c r="AB25" s="360"/>
+      <c r="AC25" s="361"/>
       <c r="AD25" s="65"/>
       <c r="AE25" s="65"/>
-      <c r="AF25" s="366"/>
-      <c r="AG25" s="368" t="s">
+      <c r="AF25" s="359"/>
+      <c r="AG25" s="360" t="s">
         <v>181</v>
       </c>
-      <c r="AH25" s="368"/>
-      <c r="AI25" s="368"/>
-      <c r="AJ25" s="368"/>
-      <c r="AK25" s="369"/>
+      <c r="AH25" s="360"/>
+      <c r="AI25" s="360"/>
+      <c r="AJ25" s="360"/>
+      <c r="AK25" s="361"/>
       <c r="AL25" s="65"/>
       <c r="AM25" s="65"/>
       <c r="AN25" s="65"/>
@@ -11533,41 +11614,41 @@
       <c r="AY25" s="65"/>
     </row>
     <row r="26" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="357"/>
-      <c r="B26" s="370"/>
-      <c r="C26" s="370"/>
-      <c r="D26" s="370"/>
-      <c r="E26" s="370"/>
-      <c r="F26" s="370"/>
-      <c r="G26" s="370"/>
-      <c r="H26" s="370"/>
-      <c r="I26" s="370"/>
-      <c r="J26" s="370"/>
-      <c r="K26" s="370"/>
-      <c r="L26" s="370"/>
-      <c r="M26" s="370"/>
-      <c r="N26" s="370"/>
-      <c r="O26" s="370"/>
-      <c r="P26" s="370"/>
-      <c r="Q26" s="370"/>
-      <c r="R26" s="370"/>
-      <c r="S26" s="370"/>
-      <c r="T26" s="370"/>
-      <c r="U26" s="371"/>
-      <c r="X26" s="361"/>
-      <c r="Y26" s="385"/>
-      <c r="Z26" s="385"/>
-      <c r="AA26" s="385"/>
-      <c r="AB26" s="385"/>
-      <c r="AC26" s="386"/>
+      <c r="A26" s="368"/>
+      <c r="B26" s="369"/>
+      <c r="C26" s="369"/>
+      <c r="D26" s="369"/>
+      <c r="E26" s="369"/>
+      <c r="F26" s="369"/>
+      <c r="G26" s="369"/>
+      <c r="H26" s="369"/>
+      <c r="I26" s="369"/>
+      <c r="J26" s="369"/>
+      <c r="K26" s="369"/>
+      <c r="L26" s="369"/>
+      <c r="M26" s="369"/>
+      <c r="N26" s="369"/>
+      <c r="O26" s="369"/>
+      <c r="P26" s="369"/>
+      <c r="Q26" s="369"/>
+      <c r="R26" s="369"/>
+      <c r="S26" s="369"/>
+      <c r="T26" s="369"/>
+      <c r="U26" s="370"/>
+      <c r="X26" s="353"/>
+      <c r="Y26" s="362"/>
+      <c r="Z26" s="362"/>
+      <c r="AA26" s="362"/>
+      <c r="AB26" s="362"/>
+      <c r="AC26" s="363"/>
       <c r="AD26" s="65"/>
       <c r="AE26" s="65"/>
-      <c r="AF26" s="361"/>
-      <c r="AG26" s="385"/>
-      <c r="AH26" s="385"/>
-      <c r="AI26" s="385"/>
-      <c r="AJ26" s="385"/>
-      <c r="AK26" s="386"/>
+      <c r="AF26" s="353"/>
+      <c r="AG26" s="362"/>
+      <c r="AH26" s="362"/>
+      <c r="AI26" s="362"/>
+      <c r="AJ26" s="362"/>
+      <c r="AK26" s="363"/>
       <c r="AL26" s="65"/>
       <c r="AM26" s="65"/>
       <c r="AN26" s="65"/>
@@ -11585,46 +11666,46 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" s="74"/>
-      <c r="B27" s="334" t="s">
+      <c r="B27" s="328" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="324"/>
-      <c r="D27" s="334" t="s">
+      <c r="C27" s="329"/>
+      <c r="D27" s="328" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="324"/>
-      <c r="F27" s="331" t="s">
+      <c r="E27" s="329"/>
+      <c r="F27" s="336" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="381"/>
+      <c r="G27" s="366"/>
       <c r="H27" s="335" t="s">
         <v>72</v>
       </c>
-      <c r="I27" s="381"/>
-      <c r="J27" s="331" t="s">
+      <c r="I27" s="366"/>
+      <c r="J27" s="336" t="s">
         <v>73</v>
       </c>
-      <c r="K27" s="381"/>
-      <c r="L27" s="331" t="s">
+      <c r="K27" s="366"/>
+      <c r="L27" s="336" t="s">
         <v>74</v>
       </c>
-      <c r="M27" s="381"/>
-      <c r="N27" s="331" t="s">
+      <c r="M27" s="366"/>
+      <c r="N27" s="336" t="s">
         <v>75</v>
       </c>
-      <c r="O27" s="381"/>
-      <c r="P27" s="331" t="s">
+      <c r="O27" s="366"/>
+      <c r="P27" s="336" t="s">
         <v>76</v>
       </c>
-      <c r="Q27" s="381"/>
-      <c r="R27" s="331" t="s">
+      <c r="Q27" s="366"/>
+      <c r="R27" s="336" t="s">
         <v>77</v>
       </c>
-      <c r="S27" s="381"/>
-      <c r="T27" s="331" t="s">
+      <c r="S27" s="366"/>
+      <c r="T27" s="336" t="s">
         <v>78</v>
       </c>
-      <c r="U27" s="381"/>
+      <c r="U27" s="366"/>
       <c r="X27" s="274"/>
       <c r="Y27" s="308" t="s">
         <v>17</v>
@@ -11820,13 +11901,13 @@
       <c r="AF29" s="306" t="s">
         <v>0</v>
       </c>
-      <c r="AG29" s="366">
+      <c r="AG29" s="359">
         <v>0.29499999999999998</v>
       </c>
-      <c r="AH29" s="367"/>
-      <c r="AI29" s="367"/>
-      <c r="AJ29" s="367"/>
-      <c r="AK29" s="351"/>
+      <c r="AH29" s="364"/>
+      <c r="AI29" s="364"/>
+      <c r="AJ29" s="364"/>
+      <c r="AK29" s="365"/>
     </row>
     <row r="30" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A30" s="96" t="s">
@@ -11894,13 +11975,13 @@
       <c r="AF30" s="306" t="s">
         <v>1</v>
       </c>
-      <c r="AG30" s="393">
+      <c r="AG30" s="356">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AH30" s="394"/>
-      <c r="AI30" s="394"/>
-      <c r="AJ30" s="394"/>
-      <c r="AK30" s="395"/>
+      <c r="AH30" s="357"/>
+      <c r="AI30" s="357"/>
+      <c r="AJ30" s="357"/>
+      <c r="AK30" s="358"/>
     </row>
     <row r="31" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A31" s="96" t="s">
@@ -11988,13 +12069,13 @@
       <c r="AF31" s="306" t="s">
         <v>2</v>
       </c>
-      <c r="AG31" s="360">
+      <c r="AG31" s="347">
         <v>0.37</v>
       </c>
-      <c r="AH31" s="362"/>
-      <c r="AI31" s="362"/>
-      <c r="AJ31" s="362"/>
-      <c r="AK31" s="352"/>
+      <c r="AH31" s="348"/>
+      <c r="AI31" s="348"/>
+      <c r="AJ31" s="348"/>
+      <c r="AK31" s="349"/>
     </row>
     <row r="32" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A32" s="96" t="s">
@@ -12062,13 +12143,13 @@
       <c r="AF32" s="306" t="s">
         <v>3</v>
       </c>
-      <c r="AG32" s="360">
+      <c r="AG32" s="347">
         <v>0.68</v>
       </c>
-      <c r="AH32" s="362"/>
-      <c r="AI32" s="362"/>
-      <c r="AJ32" s="362"/>
-      <c r="AK32" s="352"/>
+      <c r="AH32" s="348"/>
+      <c r="AI32" s="348"/>
+      <c r="AJ32" s="348"/>
+      <c r="AK32" s="349"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" s="96" t="s">
@@ -12136,13 +12217,13 @@
       <c r="AF33" s="306" t="s">
         <v>4</v>
       </c>
-      <c r="AG33" s="360">
+      <c r="AG33" s="347">
         <v>0.11899999999999999</v>
       </c>
-      <c r="AH33" s="362"/>
-      <c r="AI33" s="362"/>
-      <c r="AJ33" s="362"/>
-      <c r="AK33" s="352"/>
+      <c r="AH33" s="348"/>
+      <c r="AI33" s="348"/>
+      <c r="AJ33" s="348"/>
+      <c r="AK33" s="349"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" s="96" t="s">
@@ -12230,13 +12311,13 @@
       <c r="AF34" s="306" t="s">
         <v>5</v>
       </c>
-      <c r="AG34" s="360">
+      <c r="AG34" s="347">
         <v>0.255</v>
       </c>
-      <c r="AH34" s="362"/>
-      <c r="AI34" s="362"/>
-      <c r="AJ34" s="362"/>
-      <c r="AK34" s="352"/>
+      <c r="AH34" s="348"/>
+      <c r="AI34" s="348"/>
+      <c r="AJ34" s="348"/>
+      <c r="AK34" s="349"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" s="96" t="s">
@@ -12304,13 +12385,13 @@
       <c r="AF35" s="306" t="s">
         <v>6</v>
       </c>
-      <c r="AG35" s="360">
+      <c r="AG35" s="347">
         <v>0.72</v>
       </c>
-      <c r="AH35" s="362"/>
-      <c r="AI35" s="362"/>
-      <c r="AJ35" s="362"/>
-      <c r="AK35" s="352"/>
+      <c r="AH35" s="348"/>
+      <c r="AI35" s="348"/>
+      <c r="AJ35" s="348"/>
+      <c r="AK35" s="349"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" s="96" t="s">
@@ -12378,13 +12459,13 @@
       <c r="AF36" s="306" t="s">
         <v>7</v>
       </c>
-      <c r="AG36" s="360">
+      <c r="AG36" s="347">
         <v>0.43</v>
       </c>
-      <c r="AH36" s="362"/>
-      <c r="AI36" s="362"/>
-      <c r="AJ36" s="362"/>
-      <c r="AK36" s="352"/>
+      <c r="AH36" s="348"/>
+      <c r="AI36" s="348"/>
+      <c r="AJ36" s="348"/>
+      <c r="AK36" s="349"/>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" s="96" t="s">
@@ -12452,13 +12533,13 @@
       <c r="AF37" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="AG37" s="360">
+      <c r="AG37" s="347">
         <v>0.29399999999999998</v>
       </c>
-      <c r="AH37" s="362"/>
-      <c r="AI37" s="362"/>
-      <c r="AJ37" s="362"/>
-      <c r="AK37" s="352"/>
+      <c r="AH37" s="348"/>
+      <c r="AI37" s="348"/>
+      <c r="AJ37" s="348"/>
+      <c r="AK37" s="349"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" s="96" t="s">
@@ -12526,13 +12607,13 @@
       <c r="AF38" s="306" t="s">
         <v>9</v>
       </c>
-      <c r="AG38" s="396">
+      <c r="AG38" s="350">
         <v>0.26600000000000001</v>
       </c>
-      <c r="AH38" s="397"/>
-      <c r="AI38" s="397"/>
-      <c r="AJ38" s="397"/>
-      <c r="AK38" s="398"/>
+      <c r="AH38" s="351"/>
+      <c r="AI38" s="351"/>
+      <c r="AJ38" s="351"/>
+      <c r="AK38" s="352"/>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" s="96" t="s">
@@ -12620,13 +12701,13 @@
       <c r="AF39" s="306" t="s">
         <v>10</v>
       </c>
-      <c r="AG39" s="360">
+      <c r="AG39" s="347">
         <v>0.19900000000000001</v>
       </c>
-      <c r="AH39" s="362"/>
-      <c r="AI39" s="362"/>
-      <c r="AJ39" s="362"/>
-      <c r="AK39" s="352"/>
+      <c r="AH39" s="348"/>
+      <c r="AI39" s="348"/>
+      <c r="AJ39" s="348"/>
+      <c r="AK39" s="349"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" s="96" t="s">
@@ -12694,13 +12775,13 @@
       <c r="AF40" s="306" t="s">
         <v>11</v>
       </c>
-      <c r="AG40" s="360">
+      <c r="AG40" s="347">
         <v>0.37</v>
       </c>
-      <c r="AH40" s="362"/>
-      <c r="AI40" s="362"/>
-      <c r="AJ40" s="362"/>
-      <c r="AK40" s="352"/>
+      <c r="AH40" s="348"/>
+      <c r="AI40" s="348"/>
+      <c r="AJ40" s="348"/>
+      <c r="AK40" s="349"/>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" s="96" t="s">
@@ -12768,13 +12849,13 @@
       <c r="AF41" s="306" t="s">
         <v>12</v>
       </c>
-      <c r="AG41" s="393">
+      <c r="AG41" s="356">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="AH41" s="394"/>
-      <c r="AI41" s="394"/>
-      <c r="AJ41" s="394"/>
-      <c r="AK41" s="395"/>
+      <c r="AH41" s="357"/>
+      <c r="AI41" s="357"/>
+      <c r="AJ41" s="357"/>
+      <c r="AK41" s="358"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" s="96" t="s">
@@ -12842,13 +12923,13 @@
       <c r="AF42" s="306" t="s">
         <v>13</v>
       </c>
-      <c r="AG42" s="360">
+      <c r="AG42" s="347">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="AH42" s="362"/>
-      <c r="AI42" s="362"/>
-      <c r="AJ42" s="362"/>
-      <c r="AK42" s="352"/>
+      <c r="AH42" s="348"/>
+      <c r="AI42" s="348"/>
+      <c r="AJ42" s="348"/>
+      <c r="AK42" s="349"/>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" s="96" t="s">
@@ -12916,13 +12997,13 @@
       <c r="AF43" s="306" t="s">
         <v>14</v>
       </c>
-      <c r="AG43" s="360">
+      <c r="AG43" s="347">
         <v>0.126</v>
       </c>
-      <c r="AH43" s="362"/>
-      <c r="AI43" s="362"/>
-      <c r="AJ43" s="362"/>
-      <c r="AK43" s="352"/>
+      <c r="AH43" s="348"/>
+      <c r="AI43" s="348"/>
+      <c r="AJ43" s="348"/>
+      <c r="AK43" s="349"/>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44" s="96" t="s">
@@ -12990,13 +13071,13 @@
       <c r="AF44" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="AG44" s="396">
+      <c r="AG44" s="350">
         <v>0.16</v>
       </c>
-      <c r="AH44" s="397"/>
-      <c r="AI44" s="397"/>
-      <c r="AJ44" s="397"/>
-      <c r="AK44" s="398"/>
+      <c r="AH44" s="351"/>
+      <c r="AI44" s="351"/>
+      <c r="AJ44" s="351"/>
+      <c r="AK44" s="352"/>
     </row>
     <row r="45" spans="1:37" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="97" t="s">
@@ -13063,13 +13144,13 @@
       <c r="AF45" s="307" t="s">
         <v>16</v>
       </c>
-      <c r="AG45" s="361">
+      <c r="AG45" s="353">
         <v>0.65600000000000003</v>
       </c>
-      <c r="AH45" s="363"/>
-      <c r="AI45" s="363"/>
-      <c r="AJ45" s="363"/>
-      <c r="AK45" s="353"/>
+      <c r="AH45" s="354"/>
+      <c r="AI45" s="354"/>
+      <c r="AJ45" s="354"/>
+      <c r="AK45" s="355"/>
     </row>
     <row r="46" spans="1:37" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E46" s="116">
@@ -13109,31 +13190,29 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="AG32:AK32"/>
-    <mergeCell ref="AG33:AK33"/>
-    <mergeCell ref="AG34:AK34"/>
-    <mergeCell ref="AG35:AK35"/>
-    <mergeCell ref="AG42:AK42"/>
-    <mergeCell ref="AG43:AK43"/>
-    <mergeCell ref="AG44:AK44"/>
-    <mergeCell ref="AG45:AK45"/>
-    <mergeCell ref="AG36:AK36"/>
-    <mergeCell ref="AG37:AK37"/>
-    <mergeCell ref="AG38:AK38"/>
-    <mergeCell ref="AG39:AK39"/>
-    <mergeCell ref="AG40:AK40"/>
-    <mergeCell ref="AG41:AK41"/>
-    <mergeCell ref="AF25:AF26"/>
-    <mergeCell ref="AG25:AK26"/>
-    <mergeCell ref="AG29:AK29"/>
-    <mergeCell ref="AG30:AK30"/>
-    <mergeCell ref="AG31:AK31"/>
-    <mergeCell ref="Y25:AC26"/>
-    <mergeCell ref="X25:X26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="A25:U26"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE3:AH3"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="M1:AL2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="M3:N5"/>
     <mergeCell ref="A3:A5"/>
@@ -13150,29 +13229,31 @@
     <mergeCell ref="H3:H5"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="M1:AL2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE3:AH3"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="Y25:AC26"/>
+    <mergeCell ref="X25:X26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="A25:U26"/>
+    <mergeCell ref="AF25:AF26"/>
+    <mergeCell ref="AG25:AK26"/>
+    <mergeCell ref="AG29:AK29"/>
+    <mergeCell ref="AG30:AK30"/>
+    <mergeCell ref="AG31:AK31"/>
+    <mergeCell ref="AG43:AK43"/>
+    <mergeCell ref="AG44:AK44"/>
+    <mergeCell ref="AG45:AK45"/>
+    <mergeCell ref="AG36:AK36"/>
+    <mergeCell ref="AG37:AK37"/>
+    <mergeCell ref="AG38:AK38"/>
+    <mergeCell ref="AG39:AK39"/>
+    <mergeCell ref="AG40:AK40"/>
+    <mergeCell ref="AG41:AK41"/>
+    <mergeCell ref="AG32:AK32"/>
+    <mergeCell ref="AG33:AK33"/>
+    <mergeCell ref="AG34:AK34"/>
+    <mergeCell ref="AG35:AK35"/>
+    <mergeCell ref="AG42:AK42"/>
   </mergeCells>
   <conditionalFormatting sqref="Y29:AC29">
     <cfRule type="iconSet" priority="4">
@@ -13217,6 +13298,1051 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Q46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="231"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="399" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="399"/>
+      <c r="E2" s="399" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="399"/>
+      <c r="G2" s="399"/>
+      <c r="H2" s="399" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="400"/>
+      <c r="K2" s="400"/>
+      <c r="L2" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M2" s="401"/>
+      <c r="N2" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O2" s="401"/>
+      <c r="P2" s="401"/>
+      <c r="Q2" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="231"/>
+      <c r="B3" s="231"/>
+      <c r="C3" s="231" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="231" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="399"/>
+      <c r="F3" s="399"/>
+      <c r="G3" s="399"/>
+      <c r="H3" s="399"/>
+      <c r="J3" s="400"/>
+      <c r="K3" s="400"/>
+      <c r="L3" s="400" t="s">
+        <v>187</v>
+      </c>
+      <c r="M3" s="400" t="s">
+        <v>198</v>
+      </c>
+      <c r="N3" s="401"/>
+      <c r="O3" s="401"/>
+      <c r="P3" s="401"/>
+      <c r="Q3" s="401"/>
+    </row>
+    <row r="4" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="399" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="231" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="231">
+        <v>93</v>
+      </c>
+      <c r="D4" s="231">
+        <v>141</v>
+      </c>
+      <c r="E4" s="231" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="231" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="231" t="s">
+        <v>191</v>
+      </c>
+      <c r="H4" s="399">
+        <v>139</v>
+      </c>
+      <c r="J4" s="401" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L4" s="400"/>
+      <c r="M4" s="400"/>
+      <c r="N4" s="400"/>
+      <c r="O4" s="400"/>
+      <c r="P4" s="400"/>
+      <c r="Q4" s="401"/>
+    </row>
+    <row r="5" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="399"/>
+      <c r="B5" s="231" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="399">
+        <v>56</v>
+      </c>
+      <c r="D5" s="399"/>
+      <c r="E5" s="231" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="231" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="231" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" s="399"/>
+      <c r="J5" s="401"/>
+      <c r="K5" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L5" s="401"/>
+      <c r="M5" s="401"/>
+      <c r="N5" s="400"/>
+      <c r="O5" s="400"/>
+      <c r="P5" s="400"/>
+      <c r="Q5" s="401"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="231"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="399" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="399"/>
+      <c r="E8" s="399" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="399"/>
+      <c r="G8" s="399"/>
+      <c r="H8" s="399" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="400"/>
+      <c r="K8" s="400"/>
+      <c r="L8" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M8" s="401"/>
+      <c r="N8" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O8" s="401"/>
+      <c r="P8" s="401"/>
+      <c r="Q8" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="231"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="231" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="231" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
+      <c r="G9" s="399"/>
+      <c r="H9" s="399"/>
+      <c r="J9" s="400"/>
+      <c r="K9" s="400"/>
+      <c r="L9" s="400" t="s">
+        <v>187</v>
+      </c>
+      <c r="M9" s="400" t="s">
+        <v>198</v>
+      </c>
+      <c r="N9" s="401"/>
+      <c r="O9" s="401"/>
+      <c r="P9" s="401"/>
+      <c r="Q9" s="401"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="399" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="231" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="231">
+        <v>117</v>
+      </c>
+      <c r="D10" s="231">
+        <v>52</v>
+      </c>
+      <c r="E10" s="231" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" s="231" t="s">
+        <v>201</v>
+      </c>
+      <c r="G10" s="231" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="399">
+        <v>140</v>
+      </c>
+      <c r="J10" s="401" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L10" s="400"/>
+      <c r="M10" s="400"/>
+      <c r="N10" s="400"/>
+      <c r="O10" s="400"/>
+      <c r="P10" s="400"/>
+      <c r="Q10" s="401"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="399"/>
+      <c r="B11" s="231" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="399">
+        <v>32</v>
+      </c>
+      <c r="D11" s="399"/>
+      <c r="E11" s="231"/>
+      <c r="F11" s="231"/>
+      <c r="G11" s="231"/>
+      <c r="H11" s="399"/>
+      <c r="J11" s="401"/>
+      <c r="K11" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L11" s="401"/>
+      <c r="M11" s="401"/>
+      <c r="N11" s="400"/>
+      <c r="O11" s="400"/>
+      <c r="P11" s="400"/>
+      <c r="Q11" s="401"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="400"/>
+      <c r="B13" s="400"/>
+      <c r="C13" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="401"/>
+      <c r="E13" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="401"/>
+      <c r="G13" s="401"/>
+      <c r="H13" s="401" t="s">
+        <v>188</v>
+      </c>
+      <c r="J13" s="400"/>
+      <c r="K13" s="400"/>
+      <c r="L13" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M13" s="401"/>
+      <c r="N13" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O13" s="401"/>
+      <c r="P13" s="401"/>
+      <c r="Q13" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="400"/>
+      <c r="B14" s="400"/>
+      <c r="C14" s="400" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="400" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" s="401"/>
+      <c r="F14" s="401"/>
+      <c r="G14" s="401"/>
+      <c r="H14" s="401"/>
+      <c r="J14" s="400"/>
+      <c r="K14" s="400"/>
+      <c r="L14" s="400" t="s">
+        <v>187</v>
+      </c>
+      <c r="M14" s="400" t="s">
+        <v>199</v>
+      </c>
+      <c r="N14" s="401"/>
+      <c r="O14" s="401"/>
+      <c r="P14" s="401"/>
+      <c r="Q14" s="401"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="401" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" s="400"/>
+      <c r="D15" s="400"/>
+      <c r="E15" s="400"/>
+      <c r="F15" s="400"/>
+      <c r="G15" s="400"/>
+      <c r="H15" s="401"/>
+      <c r="J15" s="401" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L15" s="400"/>
+      <c r="M15" s="400"/>
+      <c r="N15" s="400"/>
+      <c r="O15" s="400"/>
+      <c r="P15" s="400"/>
+      <c r="Q15" s="401"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="401"/>
+      <c r="B16" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="401"/>
+      <c r="D16" s="401"/>
+      <c r="E16" s="400"/>
+      <c r="F16" s="400"/>
+      <c r="G16" s="400"/>
+      <c r="H16" s="401"/>
+      <c r="J16" s="401"/>
+      <c r="K16" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L16" s="401"/>
+      <c r="M16" s="401"/>
+      <c r="N16" s="400"/>
+      <c r="O16" s="400"/>
+      <c r="P16" s="400"/>
+      <c r="Q16" s="401"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="400"/>
+      <c r="B18" s="400"/>
+      <c r="C18" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="401"/>
+      <c r="E18" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18" s="401"/>
+      <c r="G18" s="401"/>
+      <c r="H18" s="401" t="s">
+        <v>188</v>
+      </c>
+      <c r="J18" s="400"/>
+      <c r="K18" s="400"/>
+      <c r="L18" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M18" s="401"/>
+      <c r="N18" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O18" s="401"/>
+      <c r="P18" s="401"/>
+      <c r="Q18" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="400"/>
+      <c r="B19" s="400"/>
+      <c r="C19" s="400" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" s="400" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="401"/>
+      <c r="F19" s="401"/>
+      <c r="G19" s="401"/>
+      <c r="H19" s="401"/>
+      <c r="J19" s="400"/>
+      <c r="K19" s="400"/>
+      <c r="L19" s="400" t="s">
+        <v>195</v>
+      </c>
+      <c r="M19" s="400" t="s">
+        <v>196</v>
+      </c>
+      <c r="N19" s="401"/>
+      <c r="O19" s="401"/>
+      <c r="P19" s="401"/>
+      <c r="Q19" s="401"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="401" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="400"/>
+      <c r="D20" s="400"/>
+      <c r="E20" s="400"/>
+      <c r="F20" s="400"/>
+      <c r="G20" s="400"/>
+      <c r="H20" s="401"/>
+      <c r="J20" s="401" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L20" s="400"/>
+      <c r="M20" s="400"/>
+      <c r="N20" s="400"/>
+      <c r="O20" s="400"/>
+      <c r="P20" s="400"/>
+      <c r="Q20" s="401"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="401"/>
+      <c r="B21" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="401"/>
+      <c r="D21" s="401"/>
+      <c r="E21" s="400"/>
+      <c r="F21" s="400"/>
+      <c r="G21" s="400"/>
+      <c r="H21" s="401"/>
+      <c r="J21" s="401"/>
+      <c r="K21" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L21" s="401"/>
+      <c r="M21" s="401"/>
+      <c r="N21" s="400"/>
+      <c r="O21" s="400"/>
+      <c r="P21" s="400"/>
+      <c r="Q21" s="401"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="400"/>
+      <c r="B23" s="400"/>
+      <c r="C23" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" s="401"/>
+      <c r="E23" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="401"/>
+      <c r="G23" s="401"/>
+      <c r="H23" s="401" t="s">
+        <v>188</v>
+      </c>
+      <c r="J23" s="400"/>
+      <c r="K23" s="400"/>
+      <c r="L23" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M23" s="401"/>
+      <c r="N23" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O23" s="401"/>
+      <c r="P23" s="401"/>
+      <c r="Q23" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="400"/>
+      <c r="B24" s="400"/>
+      <c r="C24" s="400" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="400" t="s">
+        <v>198</v>
+      </c>
+      <c r="E24" s="401"/>
+      <c r="F24" s="401"/>
+      <c r="G24" s="401"/>
+      <c r="H24" s="401"/>
+      <c r="J24" s="400"/>
+      <c r="K24" s="400"/>
+      <c r="L24" s="400" t="s">
+        <v>195</v>
+      </c>
+      <c r="M24" s="400" t="s">
+        <v>198</v>
+      </c>
+      <c r="N24" s="401"/>
+      <c r="O24" s="401"/>
+      <c r="P24" s="401"/>
+      <c r="Q24" s="401"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="401" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="400"/>
+      <c r="D25" s="400"/>
+      <c r="E25" s="400"/>
+      <c r="F25" s="400"/>
+      <c r="G25" s="400"/>
+      <c r="H25" s="401"/>
+      <c r="J25" s="401" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L25" s="400"/>
+      <c r="M25" s="400"/>
+      <c r="N25" s="400"/>
+      <c r="O25" s="400"/>
+      <c r="P25" s="400"/>
+      <c r="Q25" s="401"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="401"/>
+      <c r="B26" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="401"/>
+      <c r="D26" s="401"/>
+      <c r="E26" s="400"/>
+      <c r="F26" s="400"/>
+      <c r="G26" s="400"/>
+      <c r="H26" s="401"/>
+      <c r="J26" s="401"/>
+      <c r="K26" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L26" s="401"/>
+      <c r="M26" s="401"/>
+      <c r="N26" s="400"/>
+      <c r="O26" s="400"/>
+      <c r="P26" s="400"/>
+      <c r="Q26" s="401"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="400"/>
+      <c r="B28" s="400"/>
+      <c r="C28" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D28" s="401"/>
+      <c r="E28" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" s="401"/>
+      <c r="G28" s="401"/>
+      <c r="H28" s="401" t="s">
+        <v>188</v>
+      </c>
+      <c r="J28" s="400"/>
+      <c r="K28" s="400"/>
+      <c r="L28" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M28" s="401"/>
+      <c r="N28" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O28" s="401"/>
+      <c r="P28" s="401"/>
+      <c r="Q28" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="400"/>
+      <c r="B29" s="400"/>
+      <c r="C29" s="400" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="400" t="s">
+        <v>199</v>
+      </c>
+      <c r="E29" s="401"/>
+      <c r="F29" s="401"/>
+      <c r="G29" s="401"/>
+      <c r="H29" s="401"/>
+      <c r="J29" s="400"/>
+      <c r="K29" s="400"/>
+      <c r="L29" s="400" t="s">
+        <v>195</v>
+      </c>
+      <c r="M29" s="400" t="s">
+        <v>199</v>
+      </c>
+      <c r="N29" s="401"/>
+      <c r="O29" s="401"/>
+      <c r="P29" s="401"/>
+      <c r="Q29" s="401"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="401" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="400"/>
+      <c r="D30" s="400"/>
+      <c r="E30" s="400"/>
+      <c r="F30" s="400"/>
+      <c r="G30" s="400"/>
+      <c r="H30" s="401"/>
+      <c r="J30" s="401" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L30" s="400"/>
+      <c r="M30" s="400"/>
+      <c r="N30" s="400"/>
+      <c r="O30" s="400"/>
+      <c r="P30" s="400"/>
+      <c r="Q30" s="401"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="401"/>
+      <c r="B31" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="401"/>
+      <c r="D31" s="401"/>
+      <c r="E31" s="400"/>
+      <c r="F31" s="400"/>
+      <c r="G31" s="400"/>
+      <c r="H31" s="401"/>
+      <c r="J31" s="401"/>
+      <c r="K31" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L31" s="401"/>
+      <c r="M31" s="401"/>
+      <c r="N31" s="400"/>
+      <c r="O31" s="400"/>
+      <c r="P31" s="400"/>
+      <c r="Q31" s="401"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="400"/>
+      <c r="B33" s="400"/>
+      <c r="C33" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="401"/>
+      <c r="E33" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="401"/>
+      <c r="G33" s="401"/>
+      <c r="H33" s="401" t="s">
+        <v>188</v>
+      </c>
+      <c r="J33" s="400"/>
+      <c r="K33" s="400"/>
+      <c r="L33" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M33" s="401"/>
+      <c r="N33" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O33" s="401"/>
+      <c r="P33" s="401"/>
+      <c r="Q33" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="400"/>
+      <c r="B34" s="400"/>
+      <c r="C34" s="400" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="400" t="s">
+        <v>198</v>
+      </c>
+      <c r="E34" s="401"/>
+      <c r="F34" s="401"/>
+      <c r="G34" s="401"/>
+      <c r="H34" s="401"/>
+      <c r="J34" s="400"/>
+      <c r="K34" s="400"/>
+      <c r="L34" s="400" t="s">
+        <v>195</v>
+      </c>
+      <c r="M34" s="400" t="s">
+        <v>199</v>
+      </c>
+      <c r="N34" s="401"/>
+      <c r="O34" s="401"/>
+      <c r="P34" s="401"/>
+      <c r="Q34" s="401"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="401" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="400"/>
+      <c r="D35" s="400"/>
+      <c r="E35" s="400"/>
+      <c r="F35" s="400"/>
+      <c r="G35" s="400"/>
+      <c r="H35" s="401"/>
+      <c r="J35" s="401" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L35" s="400"/>
+      <c r="M35" s="400"/>
+      <c r="N35" s="400"/>
+      <c r="O35" s="400"/>
+      <c r="P35" s="400"/>
+      <c r="Q35" s="401"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="401"/>
+      <c r="B36" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="401"/>
+      <c r="D36" s="401"/>
+      <c r="E36" s="400"/>
+      <c r="F36" s="400"/>
+      <c r="G36" s="400"/>
+      <c r="H36" s="401"/>
+      <c r="J36" s="401"/>
+      <c r="K36" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L36" s="401"/>
+      <c r="M36" s="401"/>
+      <c r="N36" s="400"/>
+      <c r="O36" s="400"/>
+      <c r="P36" s="400"/>
+      <c r="Q36" s="401"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="400"/>
+      <c r="B38" s="400"/>
+      <c r="C38" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="401"/>
+      <c r="E38" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="401"/>
+      <c r="G38" s="401"/>
+      <c r="H38" s="401" t="s">
+        <v>188</v>
+      </c>
+      <c r="J38" s="400"/>
+      <c r="K38" s="400"/>
+      <c r="L38" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="M38" s="401"/>
+      <c r="N38" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="O38" s="401"/>
+      <c r="P38" s="401"/>
+      <c r="Q38" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="400"/>
+      <c r="B39" s="400"/>
+      <c r="C39" s="400" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="400" t="s">
+        <v>199</v>
+      </c>
+      <c r="E39" s="401"/>
+      <c r="F39" s="401"/>
+      <c r="G39" s="401"/>
+      <c r="H39" s="401"/>
+      <c r="J39" s="400"/>
+      <c r="K39" s="400"/>
+      <c r="L39" s="400" t="s">
+        <v>196</v>
+      </c>
+      <c r="M39" s="400" t="s">
+        <v>199</v>
+      </c>
+      <c r="N39" s="401"/>
+      <c r="O39" s="401"/>
+      <c r="P39" s="401"/>
+      <c r="Q39" s="401"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="401" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" s="400"/>
+      <c r="D40" s="400"/>
+      <c r="E40" s="400"/>
+      <c r="F40" s="400"/>
+      <c r="G40" s="400"/>
+      <c r="H40" s="401"/>
+      <c r="J40" s="401" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="L40" s="400"/>
+      <c r="M40" s="400"/>
+      <c r="N40" s="400"/>
+      <c r="O40" s="400"/>
+      <c r="P40" s="400"/>
+      <c r="Q40" s="401"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="401"/>
+      <c r="B41" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="401"/>
+      <c r="D41" s="401"/>
+      <c r="E41" s="400"/>
+      <c r="F41" s="400"/>
+      <c r="G41" s="400"/>
+      <c r="H41" s="401"/>
+      <c r="J41" s="401"/>
+      <c r="K41" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="L41" s="401"/>
+      <c r="M41" s="401"/>
+      <c r="N41" s="400"/>
+      <c r="O41" s="400"/>
+      <c r="P41" s="400"/>
+      <c r="Q41" s="401"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="400"/>
+      <c r="B43" s="400"/>
+      <c r="C43" s="401" t="s">
+        <v>184</v>
+      </c>
+      <c r="D43" s="401"/>
+      <c r="E43" s="401" t="s">
+        <v>185</v>
+      </c>
+      <c r="F43" s="401"/>
+      <c r="G43" s="401"/>
+      <c r="H43" s="401" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="400"/>
+      <c r="B44" s="400"/>
+      <c r="C44" s="400" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="400" t="s">
+        <v>196</v>
+      </c>
+      <c r="E44" s="401"/>
+      <c r="F44" s="401"/>
+      <c r="G44" s="401"/>
+      <c r="H44" s="401"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="401" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="400" t="s">
+        <v>183</v>
+      </c>
+      <c r="C45" s="400"/>
+      <c r="D45" s="400"/>
+      <c r="E45" s="400"/>
+      <c r="F45" s="400"/>
+      <c r="G45" s="400"/>
+      <c r="H45" s="401"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="401"/>
+      <c r="B46" s="400" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="401"/>
+      <c r="D46" s="401"/>
+      <c r="E46" s="400"/>
+      <c r="F46" s="400"/>
+      <c r="G46" s="400"/>
+      <c r="H46" s="401"/>
+    </row>
+  </sheetData>
+  <mergeCells count="102">
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:P39"/>
+    <mergeCell ref="Q38:Q39"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="Q40:Q41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:P34"/>
+    <mergeCell ref="Q33:Q34"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:P29"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="E2:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="118" workbookViewId="0">
@@ -13241,26 +14367,26 @@
     <row r="1" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="197"/>
-      <c r="B2" s="366" t="s">
+      <c r="B2" s="359" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="367"/>
-      <c r="D2" s="366" t="s">
+      <c r="C2" s="364"/>
+      <c r="D2" s="359" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="367"/>
-      <c r="F2" s="366" t="s">
+      <c r="E2" s="364"/>
+      <c r="F2" s="359" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="351"/>
-      <c r="H2" s="366" t="s">
+      <c r="G2" s="365"/>
+      <c r="H2" s="359" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="351"/>
-      <c r="J2" s="387" t="s">
+      <c r="I2" s="365"/>
+      <c r="J2" s="393" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="387" t="s">
+      <c r="L2" s="393" t="s">
         <v>110</v>
       </c>
     </row>
@@ -13290,9 +14416,9 @@
       <c r="I3" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="388"/>
+      <c r="J3" s="394"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="388"/>
+      <c r="L3" s="394"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="258" t="s">
@@ -14813,11 +15939,11 @@
       <c r="W36" s="4"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A37" s="334"/>
-      <c r="B37" s="334"/>
-      <c r="C37" s="334"/>
-      <c r="D37" s="334"/>
-      <c r="E37" s="334"/>
+      <c r="A37" s="328"/>
+      <c r="B37" s="328"/>
+      <c r="C37" s="328"/>
+      <c r="D37" s="328"/>
+      <c r="E37" s="328"/>
       <c r="F37" s="210"/>
       <c r="G37" s="210"/>
       <c r="H37" s="210"/>
@@ -14954,7 +16080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
@@ -14992,73 +16118,73 @@
     <row r="1" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="207"/>
-      <c r="B2" s="366" t="s">
+      <c r="B2" s="359" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="367"/>
-      <c r="D2" s="367"/>
-      <c r="E2" s="367"/>
-      <c r="F2" s="367"/>
-      <c r="G2" s="367"/>
-      <c r="H2" s="367"/>
-      <c r="I2" s="367"/>
-      <c r="J2" s="367"/>
-      <c r="K2" s="351"/>
-      <c r="L2" s="367" t="s">
+      <c r="C2" s="364"/>
+      <c r="D2" s="364"/>
+      <c r="E2" s="364"/>
+      <c r="F2" s="364"/>
+      <c r="G2" s="364"/>
+      <c r="H2" s="364"/>
+      <c r="I2" s="364"/>
+      <c r="J2" s="364"/>
+      <c r="K2" s="365"/>
+      <c r="L2" s="364" t="s">
         <v>128</v>
       </c>
-      <c r="M2" s="367"/>
-      <c r="N2" s="367"/>
-      <c r="O2" s="367"/>
-      <c r="P2" s="367"/>
-      <c r="Q2" s="367"/>
-      <c r="R2" s="367"/>
-      <c r="S2" s="367"/>
-      <c r="T2" s="367"/>
-      <c r="U2" s="351"/>
+      <c r="M2" s="364"/>
+      <c r="N2" s="364"/>
+      <c r="O2" s="364"/>
+      <c r="P2" s="364"/>
+      <c r="Q2" s="364"/>
+      <c r="R2" s="364"/>
+      <c r="S2" s="364"/>
+      <c r="T2" s="364"/>
+      <c r="U2" s="365"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="202"/>
-      <c r="B3" s="366" t="s">
+      <c r="B3" s="359" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="351"/>
-      <c r="D3" s="367" t="s">
+      <c r="C3" s="365"/>
+      <c r="D3" s="364" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="351"/>
-      <c r="F3" s="367" t="s">
+      <c r="E3" s="365"/>
+      <c r="F3" s="364" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="351"/>
-      <c r="H3" s="367" t="s">
+      <c r="G3" s="365"/>
+      <c r="H3" s="364" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="351"/>
-      <c r="J3" s="366" t="s">
+      <c r="I3" s="365"/>
+      <c r="J3" s="359" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="351"/>
-      <c r="L3" s="367" t="s">
+      <c r="K3" s="365"/>
+      <c r="L3" s="364" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="351"/>
-      <c r="N3" s="367" t="s">
+      <c r="M3" s="365"/>
+      <c r="N3" s="364" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="351"/>
-      <c r="P3" s="367" t="s">
+      <c r="O3" s="365"/>
+      <c r="P3" s="364" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="351"/>
-      <c r="R3" s="367" t="s">
+      <c r="Q3" s="365"/>
+      <c r="R3" s="364" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="351"/>
-      <c r="T3" s="367" t="s">
+      <c r="S3" s="365"/>
+      <c r="T3" s="364" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="351"/>
+      <c r="U3" s="365"/>
     </row>
     <row r="4" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="203"/>
@@ -15680,7 +16806,7 @@
         <v>141</v>
       </c>
       <c r="V12" s="283"/>
-      <c r="W12" s="392" t="s">
+      <c r="W12" s="396" t="s">
         <v>127</v>
       </c>
       <c r="X12" s="300" t="s">
@@ -15752,7 +16878,7 @@
         <v>141</v>
       </c>
       <c r="V13" s="283"/>
-      <c r="W13" s="392"/>
+      <c r="W13" s="396"/>
       <c r="X13" s="300" t="s">
         <v>156</v>
       </c>
@@ -15822,7 +16948,7 @@
         <v>141</v>
       </c>
       <c r="V14" s="284"/>
-      <c r="W14" s="392"/>
+      <c r="W14" s="396"/>
       <c r="X14" s="301" t="s">
         <v>167</v>
       </c>
@@ -15893,7 +17019,7 @@
         <v>141</v>
       </c>
       <c r="V15" s="282"/>
-      <c r="W15" s="392"/>
+      <c r="W15" s="396"/>
       <c r="X15" s="282" t="s">
         <v>157</v>
       </c>
@@ -15964,7 +17090,7 @@
         <v>141</v>
       </c>
       <c r="V16" s="280"/>
-      <c r="W16" s="392"/>
+      <c r="W16" s="396"/>
       <c r="X16" s="280" t="s">
         <v>158</v>
       </c>
@@ -16035,7 +17161,7 @@
         <v>141</v>
       </c>
       <c r="V17" s="280"/>
-      <c r="W17" s="392"/>
+      <c r="W17" s="396"/>
       <c r="X17" s="280" t="s">
         <v>159</v>
       </c>
@@ -16106,7 +17232,7 @@
         <v>141</v>
       </c>
       <c r="V18" s="280"/>
-      <c r="W18" s="392"/>
+      <c r="W18" s="396"/>
       <c r="X18" s="280" t="s">
         <v>160</v>
       </c>
@@ -16177,7 +17303,7 @@
         <v>141</v>
       </c>
       <c r="V19" s="280"/>
-      <c r="W19" s="392"/>
+      <c r="W19" s="396"/>
       <c r="X19" s="280" t="s">
         <v>162</v>
       </c>
@@ -16248,7 +17374,7 @@
         <v>146</v>
       </c>
       <c r="V20" s="280"/>
-      <c r="W20" s="392"/>
+      <c r="W20" s="396"/>
       <c r="X20" s="280" t="s">
         <v>161</v>
       </c>
@@ -16319,7 +17445,7 @@
         <v>147</v>
       </c>
       <c r="V21" s="280"/>
-      <c r="W21" s="392"/>
+      <c r="W21" s="396"/>
       <c r="X21" s="302" t="s">
         <v>163</v>
       </c>
@@ -16348,7 +17474,7 @@
       <c r="T22" s="205"/>
       <c r="U22" s="208"/>
       <c r="V22" s="280"/>
-      <c r="W22" s="392"/>
+      <c r="W22" s="396"/>
       <c r="X22" s="302" t="s">
         <v>164</v>
       </c>
@@ -16419,7 +17545,7 @@
         <v>141</v>
       </c>
       <c r="V23" s="280"/>
-      <c r="W23" s="392"/>
+      <c r="W23" s="396"/>
       <c r="X23" s="302" t="s">
         <v>165</v>
       </c>
@@ -16490,7 +17616,7 @@
         <v>141</v>
       </c>
       <c r="V24" s="280"/>
-      <c r="W24" s="392"/>
+      <c r="W24" s="396"/>
       <c r="X24" s="302" t="s">
         <v>166</v>
       </c>
@@ -16561,7 +17687,7 @@
         <v>141</v>
       </c>
       <c r="V25" s="280"/>
-      <c r="W25" s="391" t="s">
+      <c r="W25" s="395" t="s">
         <v>128</v>
       </c>
       <c r="X25" s="280" t="s">
@@ -16634,7 +17760,7 @@
         <v>141</v>
       </c>
       <c r="V26" s="280"/>
-      <c r="W26" s="391"/>
+      <c r="W26" s="395"/>
       <c r="X26" s="302" t="s">
         <v>176</v>
       </c>
@@ -16705,7 +17831,7 @@
         <v>141</v>
       </c>
       <c r="V27" s="281"/>
-      <c r="W27" s="391"/>
+      <c r="W27" s="395"/>
       <c r="X27" s="300" t="s">
         <v>177</v>
       </c>
@@ -16776,7 +17902,7 @@
         <v>141</v>
       </c>
       <c r="V28" s="283"/>
-      <c r="W28" s="391"/>
+      <c r="W28" s="395"/>
       <c r="X28" s="300" t="s">
         <v>178</v>
       </c>
@@ -16847,7 +17973,7 @@
         <v>141</v>
       </c>
       <c r="V29" s="283"/>
-      <c r="W29" s="391"/>
+      <c r="W29" s="395"/>
       <c r="X29" s="300" t="s">
         <v>179</v>
       </c>
@@ -16918,7 +18044,7 @@
         <v>141</v>
       </c>
       <c r="V30" s="283"/>
-      <c r="W30" s="391"/>
+      <c r="W30" s="395"/>
       <c r="X30" s="300" t="s">
         <v>169</v>
       </c>
@@ -16989,7 +18115,7 @@
         <v>141</v>
       </c>
       <c r="V31" s="283"/>
-      <c r="W31" s="391"/>
+      <c r="W31" s="395"/>
       <c r="X31" s="300" t="s">
         <v>170</v>
       </c>
@@ -17060,7 +18186,7 @@
         <v>141</v>
       </c>
       <c r="V32" s="283"/>
-      <c r="W32" s="391"/>
+      <c r="W32" s="395"/>
       <c r="X32" s="300" t="s">
         <v>171</v>
       </c>
@@ -17131,7 +18257,7 @@
         <v>141</v>
       </c>
       <c r="V33" s="284"/>
-      <c r="W33" s="391"/>
+      <c r="W33" s="395"/>
       <c r="X33" s="301" t="s">
         <v>172</v>
       </c>
@@ -17202,7 +18328,7 @@
         <v>141</v>
       </c>
       <c r="V34" s="282"/>
-      <c r="W34" s="391"/>
+      <c r="W34" s="395"/>
       <c r="X34" s="303" t="s">
         <v>173</v>
       </c>
@@ -17273,7 +18399,7 @@
         <v>141</v>
       </c>
       <c r="V35" s="280"/>
-      <c r="W35" s="391"/>
+      <c r="W35" s="395"/>
       <c r="X35" s="302" t="s">
         <v>174</v>
       </c>
@@ -17344,7 +18470,7 @@
         <v>141</v>
       </c>
       <c r="V36" s="280"/>
-      <c r="W36" s="391"/>
+      <c r="W36" s="395"/>
       <c r="X36" s="280" t="s">
         <v>175</v>
       </c>
@@ -17420,9 +18546,9 @@
       <c r="Y37" s="280"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A38" s="389"/>
-      <c r="B38" s="389"/>
-      <c r="C38" s="389"/>
+      <c r="A38" s="397"/>
+      <c r="B38" s="397"/>
+      <c r="C38" s="397"/>
       <c r="D38" s="286"/>
       <c r="E38" s="286"/>
       <c r="F38" s="286"/>
@@ -17447,7 +18573,7 @@
       <c r="Y38" s="280"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A39" s="390"/>
+      <c r="A39" s="398"/>
       <c r="B39" s="280"/>
       <c r="C39" s="280"/>
       <c r="D39" s="280"/>
@@ -17555,6 +18681,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="W25:W36"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
@@ -17566,11 +18697,6 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>